<commit_message>
made canonical the index
</commit_message>
<xml_diff>
--- a/input/characters.xlsx
+++ b/input/characters.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="1042">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -2280,627 +2280,663 @@
     <t xml:space="preserve">Raden, Bambang</t>
   </si>
   <si>
-    <t xml:space="preserve">Son of Antaboga. Kisah ini menceritakan tentang Raden Nagatatmala putra Batara Anantaboga yang berani melarikan Dewi Mumpuni, istri Batara Yamadipati pada saat Kahyangan Suralaya menghadapi serbuan Prabu Karungkala, penjelmaan Batara Kalakutana. Raden Nagatatmala dan Dewi Mumpuni akhirnya mendapatkan perlindungan Prabu Wisnupati di Kerajaan Purwacarita.</t>
+    <t xml:space="preserve">A son of [Antaboga] who married [Mumpuni]. She was originally married to [Yamadipati]. In one version, he had an affair with [Mumpuni]. After being caught he was sentenced to death and then killed by Batara [Guru], to be revived by his mother. In another version, he had the help of [Antaboga], who created a fake [Mumpuni] that went on pretending to be [Yamadipati]'s wife until she died suddenly. These actions were eventually discovered by his behavior was forgiven for his role in helping to defeat [Karungkala], a giant wreaking havoc in the heavens.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nagabanda, Nagapustaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nagagini, Pertiwi, Pratiwanggana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mumpuni: Antawirya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renggapura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">355-356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229-232 (Vol. VI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152-153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nakula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He is the originally the son of the Ashwini twins and Kunti. He is believed to be the most handsome amongst the Pandavas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Although nominally the son of Pandu, he is in reality an incarnation of Aswin. After the Baratayuda war, he became the rules of Mandaraka. He died a perfect death with his four borther some time after that.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadewa,Werkudara,Puntadewa,Arjuna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sayati:x; Srengganawati:x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aji Pranawajati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">234-240 (Vol. VI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narada in Hindu mythology is known as a sage who is a trilokasanjaari (the traveller of the three worlds: Heaven, Earth and the Underworld) as he is able to go to any of these three places at will. He is known as the son of Brahma. He said to have been cursed by Daksha his brother, to create conflict amongst people wherever he goes. However he is also blessed by God in way such that the conflicts that he causes will be a blessing in disguise to leads to the better good for people. He is also considered to be a great devotee of Lord Vishnu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kanekaputra. Not a God in India.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nembur_Nawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a story of a snake that entraps Bhima. He is actually Nahusha, his ancestor who has turned into a snake due to a curse by sage Agasthya. In the end Bhima help him to be redeemed from the curse and return to his normal self.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another name of Nabatnawa, the serpet defeated by Bima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NgembatLandeyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this version he is one of the Thousand Kings. But other versions have him as one of the Korawa (also known as Wikatha Boma or Boma Encik, who is killed by Werkudara, jenis boneka wayang guseng halus). // Nama serambahan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padmanaba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incarnation of Wisnu. Ketika mati masuk ke Narayana.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pancawala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prathivindhya is known as the son of Yudhishtra and Draupadi. He is also known as one of the upapandavas (sons born to each of the Pandavas and Draupadi).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Yudistira and Drupadi. He marries Pergiwati. Pergiwa marries Gatotkaca.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pandu is the son of Veda Vyasa and Ambalika. He is known to be born pale as his mother's face turned pale with fright when she met Veda Vyasa due to his appearance. He is known to be the successor of King Vichitraveerya of the Kuru house at first but goes to the forest after a curse from a sage; he hands over the throne to his brother Dhirtirashtra.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Ambalika and Abyasa. Father of the Pandawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panyarikan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">God of writing with colorful headdress. Never forgets and can keep a secret. Son of Sang Hyang Parma, grandson of Sang Hyang Taya, younger brother of Sang Hyang Wenang. // there are many versions. There is a version that says he is the son of Batara Guru, another has him as the son of Ismaya.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as sage Parasara, he is the father of Veda Vyasa. Satyavati gives birth to Veda Vyasa before her marriage as second wife of King Shantanu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father of Abiyasa, also a writer. Son of Bambang Sakri, who in turn is son of Bambang Sekutrem. Marries Durgandini and fathers Raden Dipayana (Byasa). Also fathers Rajamala and Dewi Sudesno.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Raksasa, _Lion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petruk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pracona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prabu, Kala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He wants to marry Supraba, the bidadari.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pradapa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as Vijaya, the maternal cousin of Sahadeva. Not much is mentioned about Sahadeva's wife apart from Draupadi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadewa's wife. Daughter of Tambrapeta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pragota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patih</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Ugrasena and Ken Sagupi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ken Sagupi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ugrasena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satyavati is known as a fisherman's daughter. She was initially known as Matsyagandha (she who smells of fish). Shantanu, Bhishma's father, marries her as his second wife, after his former wife Ganga (a river goddess) leaves him for breaking one of the condition set for the marriage. She gives birth to Vichitraveerya.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also known as Setyawati. Daughter of a giant, Bagaspati. She marries Narasoma (Salya). Hasil pujaan (seperti Srikandi, Drupadi dan Pandawa). Trustojumena. Pujan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulunggana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wahyu jodoh? From story wahyu kembar cakraningrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulungsari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wahyu jodoh? From story wahyu kembar cakraningrat. //mengusai premuan sebagai Pertiwi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sengkalawati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puntadewa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yudhistra, alias Dharmaraja (the King of righteousness) is the eldest of the Pandava brothers. He is the son of Yama, the god of death and justice (therefore also known as Yamadharmaraja).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oldest of the pandawa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prabu (Ramuwijaya) / Raden Ramaregawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rama is known as the King of Ayodhya. He is of the Solar lineage (Suryavamsa) which means descendents of the Sun god. The kingdom is ruled by King Dilipa followed by his son Rahu, Rahu's son Aja, Aja's son Dasharatha and Dasharatha's son Rama. This why he is sometimes addressed as Raghurama or Raghu Kula Rama (hence alluding his origins from Raghu lineage. He is born to Dasharatha and Kausalya, the first wife of Dasharatha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Dasarata and Kausalya.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramawijaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramaparasu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parashurama is known as the 7th incarnation Lord Vishnu. He is often depicted with an axe. When his father, Jamadagni gets killed by Kartaveerya Arjuna (not to be confused with Arjuna of the Pandava brothers), Parashurama goes on a mission to kill Kartaveerya and unjust kshatriyas. As a result he refuses to teach martial arts to any one who is born to the Kshatriya clan. He teaches Karna but in the end curses him when he suspects him for being a kshatriya. Although Karna is born into the warrior clan he is still not aware of it at this point of time; Karna in fact sees himself as a Sudra (lower caste) as he is brought up by charioteer Adiratha and lies to Parashurama that he is a brahmin instead; Parashurama himself is born to a brahmin father and kshatriya mother.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Resi Jamadagni and Dewi Renuka. His father asks him to kill his mother, to punish her for committing adultery with Citrarata. He makes his father promise to grant him any wish. With this he returns his borthers to human shape (they had been earlier turned into animals for refusing to kill their mother) and to bring his mother back to life. Ramaparasu is angered when Citrarata kills Jamadagni and vows to kill all kesatria warriors. Eventually Rama (from Ramayana) kills him and then becomes Dewa. // Nama mudanya Bargawa. Parasu = senjata panah.  //Moksa = mencapai kesempurnaan. // In this particular story Wahyu Kaprawiran he is already a God.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramayadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also known as Ramadi. Together with Angganjali provides Tetuka with powers to witstand attacks from Sekipu and Pracona.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">King Dahana speaks to Bantala Maruta and Ranu, he wants to marry a Citrawarsiti, daughter of King Karentegnyana in Tasikmadu.  //HY dari unsur air. //Ranu dasanama dari Tirta, Banyu, Bahni, Weh, Jahni.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subhadra, sister of Krishna and Balarama, and second wife of Arjuna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daughter of Badrahini and Basudewa. Kakrasana and Narayana are her half-brothers from a different mother. Becomes one wife of Arjuna. Also known as Sumbadra. She becomes one of Arjuna's wives.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sumbadra, Subadra, Bratajaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baladewa,Kresna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sintawaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Younger brother of Jim Dhamdharat. // Sermabahana. Rutmaka is from Dewa Ruci. // since the oral tradition has him protrayed with a Raksasa wayang, he is given the honorific Kala. But he is actually a demon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mother of Baladewa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rukmara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as Rukmi, the elder brother of Rukmini. He wanted Shishupala, on of the nephews of Lord Krishna to marry Rukmini; he did not like Krishna. He was strongly against the wedding between Krishna and Rukmini. In his battle with Krishna, he gets defeated in the end and has half of his hair and moustache shaved as a form of punishment an publich shaming.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Arya Prabu Rukma / Bisamaka and Dewi Rumbini.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rukmini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rukmini is the first wife of Lord Krishna. She is known as one of his principle wives of Lord Krishna and their first-born, Pradyumna become the crowned Prince of Dwaraka. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">First wife of Kresna. Daughter of Bismaka (Aya Prabu Rukma) and Rumbini. Has sibligs: Arya Rumkana and Dewi Rarasati (Larasati) -&gt; this one from Ken Sagupi and Arya Prabu Rukma. Kresna (Narayana), rejecting Drona. The other wives of Kresna are Jembawati (daughter of Jembawan and Trijata), Setyaboma (daughter of Ugrasena / Setyajit, king of Lesmanapura). She has three sons: Saranadewa (face of giant), Partadewa and Dewi Sitisari / Titisari.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He is the companion of Dewi Sri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JakaPupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadewa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sahadeva is known to be the most knowledgeable one amongst the Pandavas. Born to Pandu and Madri, he is said to be well versed in astrology and could understand the language of animals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youngest Pandawa, son of Madrim and Pandu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salya is the maternal uncle of Madri's sons, Nakul and Sahadeva. He is said to have accidentally ended up siding the Kauravas as Duryodhana tricks him into thinking that his accommodation at the war camp was being provided by the Pandavas when it was actually Duryodhana. As a result, due to hospitality sentiments in the Indian culture, Salya becomes unwillingly obliged to help the Kauravas. He still expressed his support for the Pandavas by demotivating Karna when he became Karna's charioteer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Mandrapati from Mandraraka and Dewi Tejawati. Gives his sister Madrim to Pandu after loosing contest for Kunti. With Setyawati, father of Burisrawa, Erawati (Baladewa), Surtikanti (Karna), Banowati (Duryudana),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narasoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandrekaswara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burisrawa,Erawati,Sutikanthi, Banowati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samba is the son of Lord Krishna. He marries Lakshmani, the daughter of Duryodhana. Although Duryodhana is against the marriage, when Balarama expresses his anger (Duryodhana speaks ill of the Yadava clan when Balarama comes to speak on behalf of Samba when he is imprisoned by Duryodhana), Duryodhana relents in the end. Samba is also seen as the main cause of destruction of the Yadava race (Krishna's clan). Many years earlier, even before the kurukshetra war, he once decided to test the power of the sages. He dresses up as a pregnant woman and went to the sages and ask whether the unborn child would be male or female. The sages, enraged by this sign of great disrespect, cast a curse saying that "she" will "give birth" to an iron material which will cause destruction the entire yadava race. An iron mace was ripped out of Samba's thigh and he pounded it and threw it into the sea. The iron dust however was tosed back to the shore of Prabasa and was turned into deadly reeds which the yadavas used to fight and kill one another with during a heated argument on whose side should they take after witnessing the Kurukshetra war.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Jembawati and Kresna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saragupita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patih of Mandura, during the reign of Basudewa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satrugna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shatrughuna is born to Sumitra, third wife of Dasharatha. He is known as the twin of Lakshmana.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twin brother of Laksmana, son of Dasarata and Sumitra.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sekipu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patih Kala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patih of Pracona.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kasipu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">285-286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sengkuni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sakuni, the maternal uncle of the Kauravas. He is plays an important in helping the Kauravas plot against the Pandavas and finds ways to defeat them, including the game of dice where the Pandavas lose their kingdom to the Kauravas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Younger brother of Gandari. [Gandara is the name of their eldest brother, not the name of a Kingdom]. Another name: Harya Suman. In reality, son of King of  Palasajenar. // some say he is the son of Gendara, some sya he is the the adik ke2 prabu Gendara.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harya Suman, Trigantalpati, Sakuni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Boar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setyaboma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satyabhama is known as the second wife and one of the Principle wives of Lord Krishna. She also faces opposition in marrying Krishna from her brother and father. She is seen as the incarnation of the Earth goddess, Bhudevi and is known for her short temper. She is of a strong disposition and even accompanies Lord Krishna during his battle with Narakasura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daughter of Prabu Setyajid / Arya Ugrasena and Dewi Wersini. Setyaki is her younger brother. She marries Narayana. With him she has Arya Styaka.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setyaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as Satyaki, he is a Yadava chieftein who helped the Pandavas in the Kurukshetra war.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also known as Wresniwara. Son of Ugrasena and Dewi Sini  / Wresini (daughter of Sanaprabawa). Marries Dewi Garbarini [ daughter of Garbanata, from Garbaruci] and has a son named Arya Sangasanga.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siti_Sendari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krishna is said to have a daughter by the name of Charumati; however she is born to Rukmini and Krishna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daughter of Kresna (Wisnu) and Dewi Pratiwi (daughter of Antaboga). // Sundari berarti bulan purnama.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siti_Sundari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pratiwi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RaraTemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not much is mentioned about Sahadeva's marriage. He is usually known as one of the husbands of Draupadi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given to Sadewa (Raden Sudamala) as wife after curing Durga back into Uma. // or after defeating Kalanjaya and Kalantaka, who are casing Endang Soka and Pradapa. //Anaknya Begawan Tambapetra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyi Pohaci Sanghyang Sri. She emerges out of an egg, which emerged out of the tears of Antaboga. The gods kill her to protect her from Batara Guru's desires.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sugriwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as the monkey king of Kishkinda and the son of the Sun god. He is the brother of Vali (Indra's son) and he helps Rama by lending the support of his Vanara army during Rama's mission to rescue his wife Sita.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also known as Guwarsa. Son of Resi Gotama [from Erraya / Grastina] and Dewi Windradi / Indradi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suparta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also known as Dananjaya.  Mretani Jim.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surabramadiraja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">King of Kraton Banon Salembag (or Simbarmanyura) who wants to marry Arimbi. // Serambahan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surati_Mantra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SuratiMatra. He is the patih of Gorawangsa.He takes care of Kangsa, the son of Maerah and Gorawangsa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surtikanthi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as Vrushali, she is the wife of Karna and the daughter of Shalya.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surtikanti. Sibling of Erawati who marries Karna, but also loves Arjuna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surya is known as the son of Aditi (Daksha's daughter) and Sage Kashyapa. He forms a part of the navagrahas (the nine planets).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">God of the son. Father of Karna, with Kunti. Son of Guru and Dewi Senggani. // Sama dengan Druwasa (perwujudnya sebagai manusia).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tambrapeta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He marries Karenumati, Princess of Chedi. Her son's name is Niramitra. Not much is mentioned about Nakula's wife apart from Draupadi. Perhaps one reason could be because Draupadi made It clear that no other wives of the Pandava should share her household in Indraprastha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begawan at Pringalas. Father of Dewi Soka,  who marries Nakula. And Pradapa (Padapa).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tambapetra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Togog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tejamantri. Brother of Semar and Guru who accompanies the antagonists.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TunggulWulung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//HY he also has his own lakon: tunggul wulung. Malihane Betara GUru. //Tidak punya prajurit, dia mengalahkan kurawa semua, dia usap jadi patung. Akhirnya karna, duryudhana takluk. Si tunggulwulung minta supaya korawa ngluruk Dwarawati. Dwarawati kalah, Kresna mencari bantuan ke Amarta. Sementara Amarta diserang juga. Bima, Gatotkaca, Antareja semua lari ke hutan. Ketemu begawan. Mereka dirubah bima jadi gajah, antasena dadi ular, gatotkaca jadi garuda. Yang merubah ini pendita yang malihane Semar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Udawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In most Indian retellings, Vasudeva is usually mentioned to have two wives Devaki and Rohini. There is no mentioning of him having children out of wedlock.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Basudewa, out of wedlock. The fourth consort of Basudewa is his mother: Ken Sagupi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ugrasena is known as the father of Kamsa and Devaki and grandson of Krishna and Balarama. He is imprisoned by Kamsa when he seizes his throne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ugrasena is the brother of Kunti, Basudewa and Ugrasena. // known as Setyajid after becoming King.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setyajit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sang Hyang Wenang. Father of Togog, Guru and Semar, with Dewi Wiranti (daughter of Rekatatama). He appears as Ruci in Dewa Ruci.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as Bhima, Hanuman's younger brother and the second Pandava.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He was wrapped in a Bungkus as a kid, he defeated Gajah Sena and got the name Bratasena as a kid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bratasena, Bima, Arya Sena, Gandawatratmaja, Panduputra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not mentioned in the Indian Mahabharata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After the Ramayana he becomes Begawan Kontawibisana. He is the son of Bisawarna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kontawibisana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Although this character is not mentioned in the Indian Mahabharata, there is a mentioning of one of the Mahabharata characters (either Karna or Arjuna) possesses Nagastra which is a weapon associated with snakes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He can take the shape of a snake. He gives a special weapon to Arjuna (Minyak Jayengkaton). Father of Asmarawati. Father of Dewi Jim Mambang, who dreams of marrying Arjuna. Arjuna gives Wilawuk's cup to his siblings so they can see the Jnvisible demonseainiesigms. //NOTE: there are differnet version about Mambang.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bambang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Arjuna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dresanala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wisnu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishnu is known as Preserver. He is the brother of Uma and brother-in-law of Lord Shiva. He is famous for his Dasavatar (10 incarnations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also known as Narayana. Son of Uma and Guru. The following are considered incarnations of him: Srimaharaja Kanwa, Resi Wisnungkara, Prabu Arjunasasrabahu, Sri Ramawijaya, Sri Batara Kresna . Prabu Airlangga, Prabu Jayabaya, Prabu Anglingdarma Prabu Ken Arok, Prabu Kertawardhana.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Tiger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wulan_Drema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wulan Derma and Dermi (female) are sons of Batara Darma. //kena kutukan incarnasi, masuk ke tubuh salah. Ulan dermi masuk ke Hagnyawati dan Ulan Derma ke tubuhnya Samba. //Harusnya ke Bomanarakasura, maka selingkuhan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wulan_Dremi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wulan Derma (male) and Dermi (female) are born to Batara Darma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yamadipati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check! Definitely in Indian version.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Yamadipati and Senggani. His wife (Mumpuni) runs away with Bambang Nagatmala (Hyang Antaboga and Dewi Suprepti). His anger makes him half giant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Guard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yamawidura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vidura is the prime minister in the court of Hastinapura. He is born to Veda Vyasa and one of the maid-servants in the Kuru. He is viewed as a wise man who provides strong support to the Pandavas for the righteousness although he is often placed in a tough spot due to his royal allegiance to the Kuru house where the Kauravas reside and to his sense of consciousness when he witnesses many instances of unfair treatment towards the Pandavas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son of Abyasa and Datri. His half brother are Pandu and Drestarasta. He marries Dewi Pamarini [daughter of Praby Dipacandra] has two sons: Sanjaya dan Yuyutsuh. // satu ayah dengan Pandu dan Destrarastra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuda_Kothi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narada in Hindu mythology is not mentioned as having a vehicle. He is known as trilokasanjaari (the traveller of the three world (Heaven, Earth and the Underworld) as he is able to go to any of these three places that he will. He is known as the son of Brahma the creator and ardent devotee of Vishnu the Preserver)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An elephant-shaped ogre that works for Nagaprasanta. After Baladewa kills Nagraprasanta, Yudakothi becomes a transport for Narada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yudhistira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrentani kingdom. saudara tua dari Arya Dananjaya, Arya Dandunwacana, jim Nakula, dan jim Sadewa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diguise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Lion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Raksasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_Raksasa1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citrasena in reality. They want to help the Korawa defeat Pandawa. They are sent by Duryudana to chase Pradapa and Endang Soka. Killed by Nakula and Sadewa in the Sudamala story.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citrarata in reality. They want to help the Korawa defeat Pandawa. They are sent by Duryudana to chase Pradapa and Endang Soka. Killed by Nakula and Sadewa in the Sudamala story.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Arjuna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Basudewa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BayuBajra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimasakti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Werkudara, Wenang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brahala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ogre shape that Kresna takes when he is angry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FakeWerkudara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weapons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Gatotkaca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godakesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pretends to be the king of Tluki seta in Semar mBagung Kayangan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He is described as the younger brother of Bomanarakasura in lakon Wahyu Topeng Waja. Also meets him in Semar Mantu (Version 2). // He appears in different lakon. He is a spriit of Desamuka.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kesawasidhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A hermitt that lives with Anoman and other hermitts. // Sebenarnya dia amemba Kresna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Lesmana_Murdaka</t>
   </si>
   <si>
     <t xml:space="preserve">Nagabanda</t>
   </si>
   <si>
-    <t xml:space="preserve">Nakula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He is the originally the son of the Ashwini twins and Kunti. He is believed to be the most handsome amongst the Pandavas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Pandu and Madrim.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narada in Hindu mythology is known as a sage who is a trilokasanjaari (the traveller of the three worlds: Heaven, Earth and the Underworld) as he is able to go to any of these three places at will. He is known as the son of Brahma. He said to have been cursed by Daksha his brother, to create conflict amongst people wherever he goes. However he is also blessed by God in way such that the conflicts that he causes will be a blessing in disguise to leads to the better good for people. He is also considered to be a great devotee of Lord Vishnu.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kanekaputra. Not a God in India.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nembur_Nawa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a story of a snake that entraps Bhima. He is actually Nahusha, his ancestor who has turned into a snake due to a curse by sage Agasthya. In the end Bhima help him to be redeemed from the curse and return to his normal self.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Another name of Nabatnawa, the serpet defeated by Bima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NgembatLandeyan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In this version he is one of the Thousand Kings. But other versions have him as one of the Korawa (also known as Wikatha Boma or Boma Encik, who is killed by Werkudara, jenis boneka wayang guseng halus). // Nama serambahan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Padmanaba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incarnation of Wisnu. Ketika mati masuk ke Narayana.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pancawala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prathivindhya is known as the son of Yudhishtra and Draupadi. He is also known as one of the upapandavas (sons born to each of the Pandavas and Draupadi).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Yudistira and Drupadi. He marries Pergiwati. Pergiwa marries Gatotkaca.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pandu is the son of Veda Vyasa and Ambalika. He is known to be born pale as his mother's face turned pale with fright when she met Veda Vyasa due to his appearance. He is known to be the successor of King Vichitraveerya of the Kuru house at first but goes to the forest after a curse from a sage; he hands over the throne to his brother Dhirtirashtra.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Ambalika and Abyasa. Father of the Pandawa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panyarikan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">God of writing with colorful headdress. Never forgets and can keep a secret. Son of Sang Hyang Parma, grandson of Sang Hyang Taya, younger brother of Sang Hyang Wenang. // there are many versions. There is a version that says he is the son of Batara Guru, another has him as the son of Ismaya.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known as sage Parasara, he is the father of Veda Vyasa. Satyavati gives birth to Veda Vyasa before her marriage as second wife of King Shantanu. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father of Abiyasa, also a writer. Son of Bambang Sakri, who in turn is son of Bambang Sekutrem. Marries Durgandini and fathers Raden Dipayana (Byasa). Also fathers Rajamala and Dewi Sudesno.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Raksasa, _Lion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petruk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pracona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prabu, Kala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He wants to marry Supraba, the bidadari.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pradapa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known as Vijaya, the maternal cousin of Sahadeva. Not much is mentioned about Sahadeva's wife apart from Draupadi.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sadewa's wife. Daughter of Tambrapeta.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pragota</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patih</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Ugrasena and Ken Sagupi.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ken Sagupi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ugrasena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satyavati is known as a fisherman's daughter. She was initially known as Matsyagandha (she who smells of fish). Shantanu, Bhishma's father, marries her as his second wife, after his former wife Ganga (a river goddess) leaves him for breaking one of the condition set for the marriage. She gives birth to Vichitraveerya.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also known as Setyawati. Daughter of a giant, Bagaspati. She marries Narasoma (Salya). Hasil pujaan (seperti Srikandi, Drupadi dan Pandawa). Trustojumena. Pujan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pulunggana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wahyu jodoh? From story wahyu kembar cakraningrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pulungsari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wahyu jodoh? From story wahyu kembar cakraningrat. //mengusai premuan sebagai Pertiwi. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sengkalawati</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puntadewa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yudhistra, alias Dharmaraja (the King of righteousness) is the eldest of the Pandava brothers. He is the son of Yama, the god of death and justice (therefore also known as Yamadharmaraja).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oldest of the pandawa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prabu (Ramuwijaya) / Raden Ramaregawa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rama is known as the King of Ayodhya. He is of the Solar lineage (Suryavamsa) which means descendents of the Sun god. The kingdom is ruled by King Dilipa followed by his son Rahu, Rahu's son Aja, Aja's son Dasharatha and Dasharatha's son Rama. This why he is sometimes addressed as Raghurama or Raghu Kula Rama (hence alluding his origins from Raghu lineage. He is born to Dasharatha and Kausalya, the first wife of Dasharatha.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Dasarata and Kausalya.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramawijaya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramaparasu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parashurama is known as the 7th incarnation Lord Vishnu. He is often depicted with an axe. When his father, Jamadagni gets killed by Kartaveerya Arjuna (not to be confused with Arjuna of the Pandava brothers), Parashurama goes on a mission to kill Kartaveerya and unjust kshatriyas. As a result he refuses to teach martial arts to any one who is born to the Kshatriya clan. He teaches Karna but in the end curses him when he suspects him for being a kshatriya. Although Karna is born into the warrior clan he is still not aware of it at this point of time; Karna in fact sees himself as a Sudra (lower caste) as he is brought up by charioteer Adiratha and lies to Parashurama that he is a brahmin instead; Parashurama himself is born to a brahmin father and kshatriya mother.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Resi Jamadagni and Dewi Renuka. His father asks him to kill his mother, to punish her for committing adultery with Citrarata. He makes his father promise to grant him any wish. With this he returns his borthers to human shape (they had been earlier turned into animals for refusing to kill their mother) and to bring his mother back to life. Ramaparasu is angered when Citrarata kills Jamadagni and vows to kill all kesatria warriors. Eventually Rama (from Ramayana) kills him and then becomes Dewa. // Nama mudanya Bargawa. Parasu = senjata panah.  //Moksa = mencapai kesempurnaan. // In this particular story Wahyu Kaprawiran he is already a God.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramayadi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also known as Ramadi. Together with Angganjali provides Tetuka with powers to witstand attacks from Sekipu and Pracona.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">King Dahana speaks to Bantala Maruta and Ranu, he wants to marry a Citrawarsiti, daughter of King Karentegnyana in Tasikmadu.  //HY dari unsur air. //Ranu dasanama dari Tirta, Banyu, Bahni, Weh, Jahni.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subhadra, sister of Krishna and Balarama, and second wife of Arjuna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daughter of Badrahini and Basudewa. Kakrasana and Narayana are her half-brothers from a different mother. Becomes one wife of Arjuna. Also known as Sumbadra. She becomes one of Arjuna's wives.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sumbadra, Subadra, Bratajaya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baladewa,Kresna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sintawaka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Younger brother of Jim Dhamdharat. // Sermabahana. Rutmaka is from Dewa Ruci. // since the oral tradition has him protrayed with a Raksasa wayang, he is given the honorific Kala. But he is actually a demon.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother of Baladewa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rukmara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known as Rukmi, the elder brother of Rukmini. He wanted Shishupala, on of the nephews of Lord Krishna to marry Rukmini; he did not like Krishna. He was strongly against the wedding between Krishna and Rukmini. In his battle with Krishna, he gets defeated in the end and has half of his hair and moustache shaved as a form of punishment an publich shaming.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Arya Prabu Rukma / Bisamaka and Dewi Rumbini.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rukmini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rukmini is the first wife of Lord Krishna. She is known as one of his principle wives of Lord Krishna and their first-born, Pradyumna become the crowned Prince of Dwaraka. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">First wife of Kresna. Daughter of Bismaka (Aya Prabu Rukma) and Rumbini. Has sibligs: Arya Rumkana and Dewi Rarasati (Larasati) -&gt; this one from Ken Sagupi and Arya Prabu Rukma. Kresna (Narayana), rejecting Drona. The other wives of Kresna are Jembawati (daughter of Jembawan and Trijata), Setyaboma (daughter of Ugrasena / Setyajit, king of Lesmanapura). She has three sons: Saranadewa (face of giant), Partadewa and Dewi Sitisari / Titisari.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sadana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He is the companion of Dewi Sri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JakaPupon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sadewa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sahadeva is known to be the most knowledgeable one amongst the Pandavas. Born to Pandu and Madri, he is said to be well versed in astrology and could understand the language of animals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Youngest Pandawa, son of Madrim and Pandu.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salya is the maternal uncle of Madri's sons, Nakul and Sahadeva. He is said to have accidentally ended up siding the Kauravas as Duryodhana tricks him into thinking that his accommodation at the war camp was being provided by the Pandavas when it was actually Duryodhana. As a result, due to hospitality sentiments in the Indian culture, Salya becomes unwillingly obliged to help the Kauravas. He still expressed his support for the Pandavas by demotivating Karna when he became Karna's charioteer. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Mandrapati from Mandraraka and Dewi Tejawati. Gives his sister Madrim to Pandu after loosing contest for Kunti. With Setyawati, father of Burisrawa, Erawati (Baladewa), Surtikanti (Karna), Banowati (Duryudana),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narasoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mandrekaswara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burisrawa,Erawati,Sutikanthi, Banowati</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samba is the son of Lord Krishna. He marries Lakshmani, the daughter of Duryodhana. Although Duryodhana is against the marriage, when Balarama expresses his anger (Duryodhana speaks ill of the Yadava clan when Balarama comes to speak on behalf of Samba when he is imprisoned by Duryodhana), Duryodhana relents in the end. Samba is also seen as the main cause of destruction of the Yadava race (Krishna's clan). Many years earlier, even before the kurukshetra war, he once decided to test the power of the sages. He dresses up as a pregnant woman and went to the sages and ask whether the unborn child would be male or female. The sages, enraged by this sign of great disrespect, cast a curse saying that "she" will "give birth" to an iron material which will cause destruction the entire yadava race. An iron mace was ripped out of Samba's thigh and he pounded it and threw it into the sea. The iron dust however was tosed back to the shore of Prabasa and was turned into deadly reeds which the yadavas used to fight and kill one another with during a heated argument on whose side should they take after witnessing the Kurukshetra war.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Jembawati and Kresna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saragupita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patih of Mandura, during the reign of Basudewa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satrugna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shatrughuna is born to Sumitra, third wife of Dasharatha. He is known as the twin of Lakshmana.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twin brother of Laksmana, son of Dasarata and Sumitra.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sekipu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patih Kala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patih of Pracona.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kasipu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">285-286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sengkuni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sakuni, the maternal uncle of the Kauravas. He is plays an important in helping the Kauravas plot against the Pandavas and finds ways to defeat them, including the game of dice where the Pandavas lose their kingdom to the Kauravas. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Younger brother of Gandari. [Gandara is the name of their eldest brother, not the name of a Kingdom]. Another name: Harya Suman. In reality, son of King of  Palasajenar. // some say he is the son of Gendara, some sya he is the the adik ke2 prabu Gendara.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harya Suman, Trigantalpati, Sakuni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Boar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setyaboma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satyabhama is known as the second wife and one of the Principle wives of Lord Krishna. She also faces opposition in marrying Krishna from her brother and father. She is seen as the incarnation of the Earth goddess, Bhudevi and is known for her short temper. She is of a strong disposition and even accompanies Lord Krishna during his battle with Narakasura.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daughter of Prabu Setyajid / Arya Ugrasena and Dewi Wersini. Setyaki is her younger brother. She marries Narayana. With him she has Arya Styaka.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setyaki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known as Satyaki, he is a Yadava chieftein who helped the Pandavas in the Kurukshetra war.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also known as Wresniwara. Son of Ugrasena and Dewi Sini  / Wresini (daughter of Sanaprabawa). Marries Dewi Garbarini [ daughter of Garbanata, from Garbaruci] and has a son named Arya Sangasanga.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siti_Sendari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krishna is said to have a daughter by the name of Charumati; however she is born to Rukmini and Krishna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daughter of Kresna (Wisnu) and Dewi Pratiwi (daughter of Antaboga). // Sundari berarti bulan purnama.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siti_Sundari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pratiwi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RaraTemon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not much is mentioned about Sahadeva's marriage. He is usually known as one of the husbands of Draupadi.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given to Sadewa (Raden Sudamala) as wife after curing Durga back into Uma. // or after defeating Kalanjaya and Kalantaka, who are casing Endang Soka and Pradapa. //Anaknya Begawan Tambapetra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nyi Pohaci Sanghyang Sri. She emerges out of an egg, which emerged out of the tears of Antaboga. The gods kill her to protect her from Batara Guru's desires.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sugriwa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known as the monkey king of Kishkinda and the son of the Sun god. He is the brother of Vali (Indra's son) and he helps Rama by lending the support of his Vanara army during Rama's mission to rescue his wife Sita.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also known as Guwarsa. Son of Resi Gotama [from Erraya / Grastina] and Dewi Windradi / Indradi.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suparta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also known as Dananjaya.  Mretani Jim.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surabramadiraja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">King of Kraton Banon Salembag (or Simbarmanyura) who wants to marry Arimbi. // Serambahan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surati_Mantra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SuratiMatra. He is the patih of Gorawangsa.He takes care of Kangsa, the son of Maerah and Gorawangsa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surtikanthi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known as Vrushali, she is the wife of Karna and the daughter of Shalya.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surtikanti. Sibling of Erawati who marries Karna, but also loves Arjuna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surya is known as the son of Aditi (Daksha's daughter) and Sage Kashyapa. He forms a part of the navagrahas (the nine planets).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">God of the son. Father of Karna, with Kunti. Son of Guru and Dewi Senggani. // Sama dengan Druwasa (perwujudnya sebagai manusia).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tambrapeta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He marries Karenumati, Princess of Chedi. Her son's name is Niramitra. Not much is mentioned about Nakula's wife apart from Draupadi. Perhaps one reason could be because Draupadi made It clear that no other wives of the Pandava should share her household in Indraprastha.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Begawan at Pringalas. Father of Dewi Soka,  who marries Nakula. And Pradapa (Padapa).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tambapetra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Togog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tejamantri. Brother of Semar and Guru who accompanies the antagonists.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TunggulWulung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//HY he also has his own lakon: tunggul wulung. Malihane Betara GUru. //Tidak punya prajurit, dia mengalahkan kurawa semua, dia usap jadi patung. Akhirnya karna, duryudhana takluk. Si tunggulwulung minta supaya korawa ngluruk Dwarawati. Dwarawati kalah, Kresna mencari bantuan ke Amarta. Sementara Amarta diserang juga. Bima, Gatotkaca, Antareja semua lari ke hutan. Ketemu begawan. Mereka dirubah bima jadi gajah, antasena dadi ular, gatotkaca jadi garuda. Yang merubah ini pendita yang malihane Semar. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Udawa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In most Indian retellings, Vasudeva is usually mentioned to have two wives Devaki and Rohini. There is no mentioning of him having children out of wedlock.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Basudewa, out of wedlock. The fourth consort of Basudewa is his mother: Ken Sagupi.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ugrasena is known as the father of Kamsa and Devaki and grandson of Krishna and Balarama. He is imprisoned by Kamsa when he seizes his throne.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ugrasena is the brother of Kunti, Basudewa and Ugrasena. // known as Setyajid after becoming King.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setyajit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wenang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sang Hyang Wenang. Father of Togog, Guru and Semar, with Dewi Wiranti (daughter of Rekatatama). He appears as Ruci in Dewa Ruci.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known as Bhima, Hanuman's younger brother and the second Pandava.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He was wrapped in a Bungkus as a kid, he defeated Gajah Sena and got the name Bratasena as a kid.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bratasena, Bima, Arya Sena, Gandawatratmaja, Panduputra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not mentioned in the Indian Mahabharata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After the Ramayana he becomes Begawan Kontawibisana. He is the son of Bisawarna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kontawibisana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Although this character is not mentioned in the Indian Mahabharata, there is a mentioning of one of the Mahabharata characters (either Karna or Arjuna) possesses Nagastra which is a weapon associated with snakes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He can take the shape of a snake. He gives a special weapon to Arjuna (Minyak Jayengkaton). Father of Asmarawati. Father of Dewi Jim Mambang, who dreams of marrying Arjuna. Arjuna gives Wilawuk's cup to his siblings so they can see the Jnvisible demonseainiesigms. //NOTE: there are differnet version about Mambang.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bambang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Arjuna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dresanala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wisnu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishnu is known as Preserver. He is the brother of Uma and brother-in-law of Lord Shiva. He is famous for his Dasavatar (10 incarnations)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also known as Narayana. Son of Uma and Guru. The following are considered incarnations of him: Srimaharaja Kanwa, Resi Wisnungkara, Prabu Arjunasasrabahu, Sri Ramawijaya, Sri Batara Kresna . Prabu Airlangga, Prabu Jayabaya, Prabu Anglingdarma Prabu Ken Arok, Prabu Kertawardhana.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Tiger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wulan_Drema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wulan Derma and Dermi (female) are sons of Batara Darma. //kena kutukan incarnasi, masuk ke tubuh salah. Ulan dermi masuk ke Hagnyawati dan Ulan Derma ke tubuhnya Samba. //Harusnya ke Bomanarakasura, maka selingkuhan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wulan_Dremi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wulan Derma (male) and Dermi (female) are born to Batara Darma.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yamadipati</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check! Definitely in Indian version.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Yamadipati and Senggani. His wife (Mumpuni) runs away with Bambang Nagatmala (Hyang Antaboga and Dewi Suprepti). His anger makes him half giant.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Guard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yamawidura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vidura is the prime minister in the court of Hastinapura. He is born to Veda Vyasa and one of the maid-servants in the Kuru. He is viewed as a wise man who provides strong support to the Pandavas for the righteousness although he is often placed in a tough spot due to his royal allegiance to the Kuru house where the Kauravas reside and to his sense of consciousness when he witnesses many instances of unfair treatment towards the Pandavas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Abyasa and Datri. His half brother are Pandu and Drestarasta. He marries Dewi Pamarini [daughter of Praby Dipacandra] has two sons: Sanjaya dan Yuyutsuh. // satu ayah dengan Pandu dan Destrarastra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yuda_Kothi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narada in Hindu mythology is not mentioned as having a vehicle. He is known as trilokasanjaari (the traveller of the three world (Heaven, Earth and the Underworld) as he is able to go to any of these three places that he will. He is known as the son of Brahma the creator and ardent devotee of Vishnu the Preserver)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An elephant-shaped ogre that works for Nagaprasanta. After Baladewa kills Nagraprasanta, Yudakothi becomes a transport for Narada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yudhistira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrentani kingdom. saudara tua dari Arya Dananjaya, Arya Dandunwacana, jim Nakula, dan jim Sadewa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diguise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lakon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Lion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Raksasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Raksasa1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citrasena in reality. They want to help the Korawa defeat Pandawa. They are sent by Duryudana to chase Pradapa and Endang Soka. Killed by Nakula and Sadewa in the Sudamala story.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citrarata in reality. They want to help the Korawa defeat Pandawa. They are sent by Duryudana to chase Pradapa and Endang Soka. Killed by Nakula and Sadewa in the Sudamala story.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Arjuna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Basudewa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BayuBajra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bimasakti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Werkudara, Wenang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brahala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ogre shape that Kresna takes when he is angry.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FakeWerkudara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weapons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Gatotkaca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godakesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pretends to be the king of Tluki seta in Semar mBagung Kayangan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He is described as the younger brother of Bomanarakasura in lakon Wahyu Topeng Waja. Also meets him in Semar Mantu (Version 2). // He appears in different lakon. He is a spriit of Desamuka.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Java?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kesawasidhi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A hermitt that lives with Anoman and other hermitts. // Sebenarnya dia amemba Kresna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Lesmana_Murdaka</t>
-  </si>
-  <si>
     <t xml:space="preserve">PrabuBandung Nagasewu</t>
   </si>
   <si>
@@ -3202,6 +3238,12 @@
   </si>
   <si>
     <t xml:space="preserve">Allows the owner to see the future.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aji Pranajawati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows the owner to never forget.</t>
   </si>
 </sst>
 </file>
@@ -3365,7 +3407,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3436,6 +3478,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -3530,46 +3576,46 @@
   <dimension ref="A1:AC148"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S73" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
-      <selection pane="bottomRight" activeCell="L84" activeCellId="0" sqref="L84"/>
+      <selection pane="bottomRight" activeCell="W86" activeCellId="0" sqref="W86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.9540816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="153.132653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="122.790816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="131.321428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="61.234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="38.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="40.5"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="34.4489795918367"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="25.7040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="66.0918367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="42.4438775510204"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="53.3469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="46.7602040816327"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="14.1479591836735"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="20.4132653061224"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.0357142857143"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="15.765306122449"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="20.734693877551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="19.765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="30" style="1" width="198.923469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="2" width="198.923469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.8520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="164.040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="131.321428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="140.607142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.4438775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="41.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.9132653061224"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="43.0918367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="36.8265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.2142857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="34.4489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="70.6275510204082"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="45.25"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="56.9132653061225"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="49.8928571428572"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="19.765306122449"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.7091836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="15.984693877551"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="16.6326530612245"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="23.0051020408163"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="22.030612244898"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1023" min="30" style="1" width="213.178571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="2" width="213.178571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7943,7 +7989,9 @@
       <c r="E83" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F83" s="3"/>
+      <c r="F83" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G83" s="1" t="s">
         <v>707</v>
       </c>
@@ -8026,7 +8074,7 @@
       <c r="X84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="4" t="s">
         <v>718</v>
       </c>
       <c r="B85" s="3"/>
@@ -8039,35 +8087,53 @@
       <c r="E85" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F85" s="3"/>
+      <c r="F85" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>720</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="I85" s="3"/>
+      <c r="I85" s="3" t="s">
+        <v>709</v>
+      </c>
       <c r="J85" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K85" s="3"/>
-      <c r="L85" s="3"/>
+      <c r="K85" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>723</v>
+      </c>
       <c r="M85" s="3"/>
-      <c r="N85" s="0"/>
+      <c r="N85" s="0" t="s">
+        <v>724</v>
+      </c>
       <c r="O85" s="0"/>
       <c r="P85" s="0"/>
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
       <c r="S85" s="0"/>
-      <c r="T85" s="0"/>
-      <c r="U85" s="0"/>
+      <c r="T85" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="U85" s="0" t="n">
+        <v>169</v>
+      </c>
       <c r="V85" s="0"/>
-      <c r="W85" s="0"/>
-      <c r="X85" s="0"/>
+      <c r="W85" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="X85" s="0" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>722</v>
+        <v>728</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>25</v>
@@ -8082,27 +8148,43 @@
         <v>28</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>723</v>
+        <v>729</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
+        <v>730</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>733</v>
+      </c>
       <c r="M86" s="3"/>
-      <c r="N86" s="0"/>
+      <c r="N86" s="0" t="s">
+        <v>191</v>
+      </c>
       <c r="O86" s="0"/>
-      <c r="P86" s="0"/>
+      <c r="P86" s="0" t="s">
+        <v>734</v>
+      </c>
       <c r="Q86" s="3"/>
       <c r="R86" s="3"/>
       <c r="S86" s="0"/>
       <c r="T86" s="0"/>
       <c r="U86" s="0"/>
       <c r="V86" s="0"/>
-      <c r="W86" s="0"/>
+      <c r="W86" s="0" t="s">
+        <v>735</v>
+      </c>
       <c r="X86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8120,10 +8202,10 @@
         <v>28</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>725</v>
+        <v>736</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>726</v>
+        <v>737</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -8149,23 +8231,23 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="18" t="s">
-        <v>727</v>
+        <v>738</v>
       </c>
       <c r="B88" s="17"/>
-      <c r="C88" s="18" t="s">
+      <c r="C88" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D88" s="18" t="s">
-        <v>728</v>
-      </c>
-      <c r="E88" s="18" t="s">
+      <c r="D88" s="19" t="s">
+        <v>739</v>
+      </c>
+      <c r="E88" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F88" s="18" t="s">
-        <v>729</v>
-      </c>
-      <c r="G88" s="18" t="s">
-        <v>730</v>
+      <c r="F88" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="G88" s="19" t="s">
+        <v>741</v>
       </c>
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
@@ -8173,21 +8255,21 @@
       <c r="K88" s="17"/>
       <c r="L88" s="17"/>
       <c r="M88" s="17"/>
-      <c r="N88" s="18"/>
-      <c r="O88" s="18"/>
-      <c r="P88" s="18"/>
+      <c r="N88" s="19"/>
+      <c r="O88" s="19"/>
+      <c r="P88" s="19"/>
       <c r="Q88" s="17"/>
-      <c r="R88" s="18"/>
-      <c r="S88" s="18"/>
-      <c r="T88" s="19"/>
-      <c r="U88" s="18"/>
-      <c r="V88" s="18"/>
-      <c r="W88" s="18"/>
-      <c r="X88" s="18"/>
+      <c r="R88" s="19"/>
+      <c r="S88" s="19"/>
+      <c r="T88" s="20"/>
+      <c r="U88" s="19"/>
+      <c r="V88" s="19"/>
+      <c r="W88" s="19"/>
+      <c r="X88" s="19"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>731</v>
+        <v>742</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="1" t="s">
@@ -8201,7 +8283,7 @@
       </c>
       <c r="F89" s="3"/>
       <c r="G89" s="1" t="s">
-        <v>732</v>
+        <v>743</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -8214,7 +8296,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>733</v>
+        <v>744</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="1" t="s">
@@ -8230,7 +8312,7 @@
         <v>209</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>734</v>
+        <v>745</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
@@ -8243,7 +8325,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>735</v>
+        <v>746</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>25</v>
@@ -8258,10 +8340,10 @@
         <v>62</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>736</v>
+        <v>747</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>737</v>
+        <v>748</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -8289,10 +8371,10 @@
         <v>28</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>738</v>
+        <v>749</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>739</v>
+        <v>750</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -8305,7 +8387,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>740</v>
+        <v>751</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="1" t="s">
@@ -8321,7 +8403,7 @@
         <v>209</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>741</v>
+        <v>752</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -8347,10 +8429,10 @@
         <v>28</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>742</v>
+        <v>753</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -8359,13 +8441,13 @@
       <c r="L94" s="3"/>
       <c r="M94" s="3"/>
       <c r="Q94" s="1" t="s">
-        <v>744</v>
+        <v>755</v>
       </c>
       <c r="T94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>745</v>
+        <v>756</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>173</v>
@@ -8392,14 +8474,14 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>746</v>
+        <v>757</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>747</v>
+        <v>758</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>62</v>
@@ -8408,7 +8490,7 @@
         <v>209</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>748</v>
+        <v>759</v>
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
@@ -8421,7 +8503,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>749</v>
+        <v>760</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="1" t="s">
@@ -8434,10 +8516,10 @@
         <v>28</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>750</v>
+        <v>761</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -8450,14 +8532,14 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>752</v>
+        <v>763</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>753</v>
+        <v>764</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>62</v>
@@ -8466,14 +8548,14 @@
         <v>209</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>754</v>
+        <v>765</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="1" t="s">
-        <v>755</v>
+        <v>766</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>756</v>
+        <v>767</v>
       </c>
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
@@ -8496,10 +8578,10 @@
         <v>28</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>757</v>
+        <v>768</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>758</v>
+        <v>769</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
@@ -8512,7 +8594,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>759</v>
+        <v>770</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="1" t="s">
@@ -8528,7 +8610,7 @@
         <v>209</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>760</v>
+        <v>771</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -8541,7 +8623,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>761</v>
+        <v>772</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="1" t="s">
@@ -8557,7 +8639,7 @@
         <v>209</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>762</v>
+        <v>773</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
@@ -8566,13 +8648,13 @@
       <c r="L101" s="3"/>
       <c r="M101" s="3"/>
       <c r="Q101" s="1" t="s">
-        <v>763</v>
+        <v>774</v>
       </c>
       <c r="T101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>764</v>
+        <v>775</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>25</v>
@@ -8587,10 +8669,10 @@
         <v>28</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>765</v>
+        <v>776</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>766</v>
+        <v>777</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -8610,19 +8692,19 @@
         <v>26</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>768</v>
+        <v>779</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>769</v>
+        <v>780</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>770</v>
+        <v>781</v>
       </c>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
@@ -8634,7 +8716,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>771</v>
+        <v>782</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="1" t="s">
@@ -8647,10 +8729,10 @@
         <v>28</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>772</v>
+        <v>783</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>773</v>
+        <v>784</v>
       </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
@@ -8663,7 +8745,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>774</v>
+        <v>785</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="1" t="s">
@@ -8679,7 +8761,7 @@
         <v>209</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>775</v>
+        <v>786</v>
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -8692,7 +8774,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>776</v>
+        <v>787</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="1" t="s">
@@ -8708,7 +8790,7 @@
         <v>209</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>777</v>
+        <v>788</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -8734,13 +8816,13 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>778</v>
+        <v>789</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>779</v>
+        <v>790</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>780</v>
+        <v>791</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>158</v>
@@ -8749,14 +8831,14 @@
         <v>188</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>781</v>
+        <v>792</v>
       </c>
       <c r="L107" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M107" s="3"/>
       <c r="Q107" s="1" t="s">
-        <v>782</v>
+        <v>793</v>
       </c>
       <c r="T107" s="0"/>
     </row>
@@ -8778,7 +8860,7 @@
         <v>209</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>783</v>
+        <v>794</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -8806,7 +8888,7 @@
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="1" t="s">
-        <v>784</v>
+        <v>795</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
@@ -8820,7 +8902,7 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>785</v>
+        <v>796</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="1" t="s">
@@ -8833,10 +8915,10 @@
         <v>28</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>786</v>
+        <v>797</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>787</v>
+        <v>798</v>
       </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
@@ -8848,7 +8930,7 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>788</v>
+        <v>799</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="1" t="s">
@@ -8861,10 +8943,10 @@
         <v>28</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>789</v>
+        <v>800</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>790</v>
+        <v>801</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
@@ -8876,7 +8958,7 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>791</v>
+        <v>802</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="1" t="s">
@@ -8890,7 +8972,7 @@
       </c>
       <c r="F112" s="3"/>
       <c r="G112" s="1" t="s">
-        <v>792</v>
+        <v>803</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -8898,13 +8980,13 @@
       <c r="L112" s="3"/>
       <c r="M112" s="3"/>
       <c r="Q112" s="1" t="s">
-        <v>793</v>
+        <v>804</v>
       </c>
       <c r="T112" s="0"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>794</v>
+        <v>805</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>25</v>
@@ -8919,10 +9001,10 @@
         <v>28</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>795</v>
+        <v>806</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>796</v>
+        <v>807</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
@@ -8947,32 +9029,32 @@
         <v>28</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>797</v>
+        <v>808</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>798</v>
+        <v>809</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>799</v>
+        <v>810</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>669</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>800</v>
+        <v>811</v>
       </c>
       <c r="L114" s="1" t="s">
         <v>433</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>801</v>
+        <v>812</v>
       </c>
       <c r="Q114" s="3"/>
       <c r="T114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>802</v>
+        <v>813</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="1" t="s">
@@ -8985,10 +9067,10 @@
         <v>28</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>803</v>
+        <v>814</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>804</v>
+        <v>815</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
@@ -8999,14 +9081,14 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>805</v>
+        <v>816</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>753</v>
+        <v>764</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>62</v>
@@ -9015,7 +9097,7 @@
         <v>209</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>806</v>
+        <v>817</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -9026,7 +9108,7 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>807</v>
+        <v>818</v>
       </c>
       <c r="B117" s="3"/>
       <c r="C117" s="1" t="s">
@@ -9039,10 +9121,10 @@
         <v>28</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>808</v>
+        <v>819</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>809</v>
+        <v>820</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -9053,14 +9135,14 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>810</v>
+        <v>821</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>811</v>
+        <v>822</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>62</v>
@@ -9069,17 +9151,17 @@
         <v>209</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>812</v>
+        <v>823</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>813</v>
+        <v>824</v>
       </c>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="M118" s="3"/>
       <c r="Q118" s="3"/>
       <c r="T118" s="1" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9093,7 +9175,7 @@
         <v>88</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>815</v>
+        <v>826</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>62</v>
@@ -9110,7 +9192,7 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>816</v>
+        <v>827</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>242</v>
@@ -9119,30 +9201,30 @@
         <v>26</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>753</v>
+        <v>764</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>817</v>
+        <v>828</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>818</v>
+        <v>829</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>819</v>
+        <v>830</v>
       </c>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="M120" s="3"/>
       <c r="Q120" s="1" t="s">
-        <v>820</v>
+        <v>831</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>821</v>
+        <v>832</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="1" t="s">
@@ -9155,10 +9237,10 @@
         <v>28</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>822</v>
+        <v>833</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>823</v>
+        <v>834</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -9168,7 +9250,7 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>824</v>
+        <v>835</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>25</v>
@@ -9183,10 +9265,10 @@
         <v>28</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>825</v>
+        <v>836</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>826</v>
+        <v>837</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -9196,7 +9278,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>827</v>
+        <v>838</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>25</v>
@@ -9211,28 +9293,28 @@
         <v>28</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>828</v>
+        <v>839</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>829</v>
+        <v>840</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>830</v>
+        <v>841</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>831</v>
+        <v>842</v>
       </c>
       <c r="J123" s="3" t="s">
         <v>189</v>
       </c>
       <c r="M123" s="3"/>
       <c r="Q123" s="1" t="s">
-        <v>832</v>
+        <v>843</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>833</v>
+        <v>844</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="1" t="s">
@@ -9245,10 +9327,10 @@
         <v>62</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>834</v>
+        <v>845</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>835</v>
+        <v>846</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -9258,7 +9340,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>836</v>
+        <v>847</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="1" t="s">
@@ -9274,19 +9356,19 @@
         <v>209</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>837</v>
+        <v>848</v>
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="M125" s="3"/>
       <c r="Q125" s="1" t="s">
-        <v>832</v>
+        <v>843</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>838</v>
+        <v>849</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="1" t="s">
@@ -9299,10 +9381,10 @@
         <v>28</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>839</v>
+        <v>850</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>840</v>
+        <v>851</v>
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
@@ -9312,14 +9394,14 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>841</v>
+        <v>852</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="1" t="s">
         <v>362</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>842</v>
+        <v>853</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>62</v>
@@ -9328,7 +9410,7 @@
         <v>209</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>843</v>
+        <v>854</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
@@ -9338,7 +9420,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>844</v>
+        <v>855</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="1" t="s">
@@ -9354,7 +9436,7 @@
         <v>209</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>845</v>
+        <v>856</v>
       </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
@@ -9364,14 +9446,14 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>846</v>
+        <v>857</v>
       </c>
       <c r="B129" s="3"/>
       <c r="C129" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>811</v>
+        <v>822</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>62</v>
@@ -9380,7 +9462,7 @@
         <v>209</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>847</v>
+        <v>858</v>
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
@@ -9390,7 +9472,7 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>848</v>
+        <v>859</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="1" t="s">
@@ -9403,10 +9485,10 @@
         <v>28</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>849</v>
+        <v>860</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>850</v>
+        <v>861</v>
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
@@ -9429,10 +9511,10 @@
         <v>28</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>851</v>
+        <v>862</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>852</v>
+        <v>863</v>
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
@@ -9442,7 +9524,7 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>853</v>
+        <v>864</v>
       </c>
       <c r="B132" s="3"/>
       <c r="C132" s="1" t="s">
@@ -9455,13 +9537,13 @@
         <v>62</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>854</v>
+        <v>865</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>855</v>
+        <v>866</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>856</v>
+        <v>867</v>
       </c>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
@@ -9470,7 +9552,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>857</v>
+        <v>868</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>173</v>
@@ -9486,7 +9568,7 @@
         <v>209</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>858</v>
+        <v>869</v>
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
@@ -9496,7 +9578,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>859</v>
+        <v>870</v>
       </c>
       <c r="B134" s="3"/>
       <c r="C134" s="1" t="s">
@@ -9512,7 +9594,7 @@
         <v>209</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>860</v>
+        <v>871</v>
       </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
@@ -9522,23 +9604,23 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>861</v>
+        <v>872</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>753</v>
+        <v>764</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>862</v>
+        <v>873</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>863</v>
+        <v>874</v>
       </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
@@ -9548,7 +9630,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>756</v>
+        <v>767</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="1" t="s">
@@ -9561,13 +9643,13 @@
         <v>28</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>864</v>
+        <v>875</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>865</v>
+        <v>876</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>866</v>
+        <v>877</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -9576,7 +9658,7 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>867</v>
+        <v>878</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="1" t="s">
@@ -9592,7 +9674,7 @@
         <v>209</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>868</v>
+        <v>879</v>
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
@@ -9617,13 +9699,13 @@
         <v>28</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>869</v>
+        <v>880</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>870</v>
+        <v>881</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>871</v>
+        <v>882</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -9647,13 +9729,13 @@
         <v>62</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>872</v>
+        <v>883</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>873</v>
+        <v>884</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>874</v>
+        <v>885</v>
       </c>
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
@@ -9675,10 +9757,10 @@
         <v>62</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>875</v>
+        <v>886</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>876</v>
+        <v>887</v>
       </c>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
@@ -9698,19 +9780,19 @@
         <v>26</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>877</v>
+        <v>888</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>872</v>
+        <v>883</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>878</v>
+        <v>889</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>879</v>
+        <v>890</v>
       </c>
       <c r="J141" s="1" t="s">
         <v>33</v>
@@ -9719,7 +9801,7 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>880</v>
+        <v>891</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>88</v>
@@ -9731,18 +9813,18 @@
         <v>28</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>881</v>
+        <v>892</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>882</v>
+        <v>893</v>
       </c>
       <c r="Q142" s="1" t="s">
-        <v>883</v>
+        <v>894</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>884</v>
+        <v>895</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>88</v>
@@ -9754,16 +9836,16 @@
         <v>62</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>872</v>
+        <v>883</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>885</v>
+        <v>896</v>
       </c>
       <c r="Q143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>886</v>
+        <v>897</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>88</v>
@@ -9775,16 +9857,16 @@
         <v>62</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>872</v>
+        <v>883</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>887</v>
+        <v>898</v>
       </c>
       <c r="Q144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>888</v>
+        <v>899</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>88</v>
@@ -9796,18 +9878,18 @@
         <v>28</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>889</v>
+        <v>900</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>890</v>
+        <v>901</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>891</v>
+        <v>902</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>892</v>
+        <v>903</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>26</v>
@@ -9819,35 +9901,35 @@
         <v>28</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>893</v>
+        <v>904</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>894</v>
+        <v>905</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>895</v>
+        <v>906</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>897</v>
+        <v>908</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>898</v>
+        <v>909</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>899</v>
+        <v>910</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>362</v>
@@ -9859,7 +9941,7 @@
         <v>62</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>900</v>
+        <v>911</v>
       </c>
     </row>
   </sheetData>
@@ -9890,37 +9972,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="101.622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="80.5612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="67.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="2" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="108.857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="86.1785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="72.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="2" width="29.9132653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>901</v>
+        <v>912</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>902</v>
+        <v>913</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>903</v>
+        <v>914</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>904</v>
+        <v>915</v>
       </c>
       <c r="F1" s="3"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>820</v>
+        <v>831</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>816</v>
+        <v>827</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9930,10 +10012,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>891</v>
+        <v>902</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>888</v>
+        <v>899</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -9943,7 +10025,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>905</v>
+        <v>916</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>51</v>
@@ -9956,7 +10038,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>906</v>
+        <v>917</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>51</v>
@@ -9969,7 +10051,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>907</v>
+        <v>918</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>304</v>
@@ -9995,10 +10077,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>883</v>
+        <v>894</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>880</v>
+        <v>891</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -10018,7 +10100,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>908</v>
+        <v>919</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10033,12 +10115,12 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>909</v>
+        <v>920</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>910</v>
+        <v>921</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>147</v>
@@ -10062,7 +10144,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>911</v>
+        <v>922</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>226</v>
@@ -10074,7 +10156,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>912</v>
+        <v>923</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>104</v>
@@ -10085,10 +10167,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>913</v>
+        <v>924</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>914</v>
+        <v>925</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -10096,23 +10178,23 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>915</v>
+        <v>926</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>189</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2" t="s">
-        <v>916</v>
+        <v>927</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>918</v>
+        <v>929</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -10120,7 +10202,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>919</v>
+        <v>930</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>467</v>
@@ -10131,14 +10213,14 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>920</v>
+        <v>931</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
-        <v>921</v>
+        <v>932</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -10151,16 +10233,16 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="1" t="s">
-        <v>922</v>
+        <v>933</v>
       </c>
       <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>793</v>
+        <v>804</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>791</v>
+        <v>802</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -10176,7 +10258,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2" t="s">
-        <v>923</v>
+        <v>934</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10189,25 +10271,25 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2" t="s">
-        <v>923</v>
+        <v>934</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>924</v>
+        <v>935</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>189</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="1" t="s">
-        <v>925</v>
+        <v>936</v>
       </c>
       <c r="F24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="s">
-        <v>926</v>
+      <c r="A25" s="21" t="s">
+        <v>937</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>33</v>
@@ -10218,7 +10300,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>721</v>
+        <v>938</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>718</v>
@@ -10235,14 +10317,14 @@
         <v>107</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>927</v>
+        <v>939</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>928</v>
+        <v>940</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>361</v>
@@ -10259,17 +10341,17 @@
         <v>108</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>929</v>
+        <v>941</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>832</v>
+        <v>843</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>930</v>
+        <v>942</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -10286,10 +10368,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>763</v>
+        <v>774</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>761</v>
+        <v>772</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -10306,19 +10388,19 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>782</v>
+        <v>793</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>931</v>
+        <v>943</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>932</v>
+        <v>944</v>
       </c>
       <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>933</v>
+        <v>945</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
@@ -10348,12 +10430,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="13.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="13.8214285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>934</v>
+        <v>946</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>7</v>
@@ -10367,33 +10449,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>935</v>
+        <v>947</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>936</v>
+        <v>948</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>937</v>
+        <v>949</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>938</v>
+        <v>950</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="3" t="s">
-        <v>939</v>
+        <v>951</v>
       </c>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>940</v>
+        <v>952</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="3" t="s">
-        <v>941</v>
+        <v>953</v>
       </c>
       <c r="D4" s="0"/>
     </row>
@@ -10402,19 +10484,19 @@
         <v>496</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>942</v>
+        <v>954</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
       <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>944</v>
+        <v>956</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>945</v>
+        <v>957</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" s="0"/>
@@ -10430,7 +10512,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>946</v>
+        <v>958</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -10448,10 +10530,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>821</v>
+        <v>832</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>756</v>
+        <v>767</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10459,7 +10541,7 @@
         <v>660</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>947</v>
+        <v>959</v>
       </c>
     </row>
   </sheetData>
@@ -10486,16 +10568,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="19.765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="B1" s="3" t="s">
-        <v>948</v>
+        <v>960</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>949</v>
+        <v>961</v>
       </c>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
@@ -10508,13 +10590,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>950</v>
+        <v>962</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>950</v>
+        <v>962</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>951</v>
+        <v>963</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
@@ -10524,7 +10606,7 @@
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="W2" s="3" t="s">
-        <v>950</v>
+        <v>962</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10553,7 +10635,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>952</v>
+        <v>964</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0"/>
@@ -10567,7 +10649,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>953</v>
+        <v>965</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0"/>
@@ -10581,7 +10663,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>954</v>
+        <v>966</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
@@ -10595,7 +10677,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>955</v>
+        <v>967</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
@@ -10604,18 +10686,18 @@
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="J8" s="3" t="s">
-        <v>956</v>
+        <v>968</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>957</v>
+        <v>969</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>958</v>
+        <v>970</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>959</v>
+        <v>971</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
@@ -10624,21 +10706,21 @@
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="J9" s="3" t="s">
-        <v>960</v>
+        <v>972</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>961</v>
+        <v>973</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>962</v>
+        <v>974</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>963</v>
+        <v>975</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>964</v>
+        <v>976</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
@@ -10646,18 +10728,18 @@
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="J10" s="3" t="s">
-        <v>965</v>
+        <v>977</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>966</v>
+        <v>978</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>967</v>
+        <v>979</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>968</v>
+        <v>980</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -10666,18 +10748,18 @@
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="J11" s="3" t="s">
-        <v>969</v>
+        <v>981</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>970</v>
+        <v>982</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>971</v>
+        <v>983</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>972</v>
+        <v>984</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
@@ -10686,21 +10768,21 @@
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="J12" s="0" t="s">
-        <v>973</v>
+        <v>985</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>975</v>
+        <v>987</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>976</v>
+        <v>988</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>977</v>
+        <v>989</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
@@ -10708,21 +10790,21 @@
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="J13" s="0" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>979</v>
+        <v>991</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>980</v>
+        <v>992</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>981</v>
+        <v>993</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>982</v>
+        <v>994</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
@@ -10731,10 +10813,10 @@
       <c r="G14" s="0"/>
       <c r="J14" s="0"/>
       <c r="L14" s="3" t="s">
-        <v>983</v>
+        <v>995</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>984</v>
+        <v>996</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10751,7 +10833,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>985</v>
+        <v>997</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -10760,13 +10842,13 @@
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="J16" s="3" t="s">
-        <v>986</v>
+        <v>998</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>987</v>
+        <v>999</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>988</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10778,18 +10860,18 @@
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="J17" s="3" t="s">
-        <v>989</v>
+        <v>1001</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>990</v>
+        <v>1002</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>991</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>992</v>
+        <v>1004</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -10798,15 +10880,15 @@
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="J18" s="3" t="s">
-        <v>993</v>
+        <v>1005</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>994</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>995</v>
+        <v>1007</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
@@ -10815,7 +10897,7 @@
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
       <c r="J19" s="3" t="s">
-        <v>996</v>
+        <v>1008</v>
       </c>
       <c r="L19" s="0"/>
     </row>
@@ -10831,7 +10913,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>997</v>
+        <v>1009</v>
       </c>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -10853,7 +10935,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>998</v>
+        <v>1010</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -10865,10 +10947,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>999</v>
+        <v>1011</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1000</v>
+        <v>1012</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
@@ -10876,7 +10958,7 @@
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
       <c r="L24" s="3" t="s">
-        <v>1001</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10888,15 +10970,15 @@
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
       <c r="L25" s="3" t="s">
-        <v>1002</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>1003</v>
+        <v>1015</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1004</v>
+        <v>1016</v>
       </c>
       <c r="C26" s="0"/>
       <c r="D26" s="0"/>
@@ -10904,7 +10986,7 @@
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
       <c r="L26" s="3" t="s">
-        <v>1005</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10916,12 +10998,12 @@
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="L27" s="3" t="s">
-        <v>1006</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>1007</v>
+        <v>1019</v>
       </c>
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
@@ -10930,7 +11012,7 @@
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
       <c r="L28" s="3" t="s">
-        <v>1008</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10952,7 +11034,7 @@
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
       <c r="L30" s="3" t="s">
-        <v>1009</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10964,7 +11046,7 @@
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="L31" s="3" t="s">
-        <v>1010</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10976,7 +11058,7 @@
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
       <c r="L32" s="3" t="s">
-        <v>1011</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10988,7 +11070,7 @@
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="L33" s="3" t="s">
-        <v>1012</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11000,38 +11082,38 @@
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>
       <c r="L34" s="3" t="s">
-        <v>1013</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>952</v>
+        <v>964</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>954</v>
+        <v>966</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>953</v>
+        <v>965</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>968</v>
+        <v>980</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1014</v>
+        <v>1026</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1003</v>
+        <v>1015</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>1015</v>
+        <v>1027</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>1016</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L36" s="3" t="s">
-        <v>1017</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>
@@ -11058,7 +11140,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11066,15 +11148,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1018</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1019</v>
+        <v>1031</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1020</v>
+        <v>1032</v>
       </c>
     </row>
   </sheetData>
@@ -11093,15 +11175,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11109,10 +11191,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1021</v>
+        <v>1033</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1022</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11120,7 +11202,7 @@
         <v>588</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1023</v>
+        <v>1035</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>584</v>
@@ -11128,10 +11210,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1024</v>
+        <v>1036</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1025</v>
+        <v>1037</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>189</v>
@@ -11139,13 +11221,21 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1026</v>
+        <v>1038</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1027</v>
+        <v>1039</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>1041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new pics and character info
</commit_message>
<xml_diff>
--- a/input/characters.xlsx
+++ b/input/characters.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="1377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="1387">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">Wahyu Hidayat, Wahyu Cakraningrat</t>
   </si>
   <si>
-    <t xml:space="preserve">Yogyakarta: Sedet, Pedasih, Kanyut; Surakarta: Bontit, Banjed, Brebes, Jayenggati, Kanyut, Malatsih, Mangu, Mriwis, Panji, Rangkung, Bulus</t>
+    <t xml:space="preserve">Yogyakarta: Sedet, Padasih, Kanyut; Surakarta: Bontit, Banjed, Brebes, Jayenggati, Kanyut, Malatsih, Mangu, Mriwis, Panji, Rangkung, Bulus</t>
   </si>
   <si>
     <t xml:space="preserve">18-20</t>
@@ -523,7 +523,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Wilawuk], a demon king. She is also known as Jimambang and marries [Arjuna]. The /Ensiklopedi Wayang Purwa/ describes Asmarawati as the daughter of Prabu [Suryaasmara] and the wife of Bambang [Sumitra], [Arjuna]'s son. The same source describes Jimambang as a separate character.</t>
+      <t xml:space="preserve">Wilawuk], a demon king. She is also known as Jim_Mambang and marries [Arjuna]. The /Ensiklopedi Wayang Purwa/ describes Asmarawati as the daughter of Prabu [Suryaasmara] and the wife of Bambang [Sumitra], [Arjuna]'s son. The same source describes Jim_Mambang as a separate character.</t>
     </r>
   </si>
   <si>
@@ -3784,7 +3784,7 @@
     <t xml:space="preserve">Lindhu</t>
   </si>
   <si>
-    <t xml:space="preserve">He is the younger brother of Ravana. In the Indian Ramayana, he is a giant, not a human. </t>
+    <t xml:space="preserve">Vibisana is the younger brother of Ravana. In the Indian Ramayana, he is a giant, not a human. </t>
   </si>
   <si>
     <t xml:space="preserve">He is the younger brother of [Desamuka]. He is the only one who has born with human face (this is different in India). Before [Rama]'s attack to Alengka, he defected to [Rama]'s side, providing vital information on the weaknesses of Alengka's army. His role is controversial – is he noble since he defected? Or should he have stayed to fight for his land, as [Kumbakarna] did? There are multiple opinions on this, which are explored differently by various dalang. After [Desamuka] was killed, Wibisana became king of Alengka, which was thereafter known as Singgelapura. He then received [Rama]'s advice on kingship, in the form of the Hastabrata, a philosophical treaty on statehood. After the Ramayana, he was known as Begawan Kunta Wibisana. He eventually abdicated in favor of his son [Dentawilukrama], and then achieved perfect death.</t>
@@ -3811,24 +3811,70 @@
     <t xml:space="preserve">288-289</t>
   </si>
   <si>
-    <t xml:space="preserve">Although this character is not mentioned in the Indian Mahabharata, there is a mentioning of one of the Mahabharata characters (either Karna or Arjuna) possesses Nagastra which is a weapon associated with snakes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He can take the shape of a snake. He gives a special weapon to Arjuna (Minyak Jayengkaton). Father of Asmarawati. Father of Dewi Jim Mambang, who dreams of marrying Arjuna. Arjuna gives Wilawuk's cup to his siblings so they can see the Jnvisible demonseainiesigms. //NOTE: there are differnet version about Mambang.</t>
+    <t xml:space="preserve">Not mentioned in the Indian Mahabharata</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">He can take the shape of a winged snake. He gives a special weapon to Arjuna (Minyak Jayengkaton). He is the favter of [Asmarawati], who is somtes said to be another name of Dewi Jimambang, who dreams of marrying Arjuna. Arjuna gives Wilawuk's cup to his siblings so they can see the invisible demons. There are differnet version about Jimambang. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">According to /Babad Wanamarta/, she is the daughter of Begawan </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF00000A"/>
+        <rFont val="FreeSans"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">WilawukThe /Ensiklopedi Wayang Purwa/ describes Asmarawati as the daughter of Prabu [Suryaasmara] and the wife of Bambang [Sumitra], [Arjuna]'s son. The same source describes Jim_Mambang as a separate character.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilwuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenga_Jayengkaton, Watu_Tempuru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1132-1133</t>
   </si>
   <si>
     <t xml:space="preserve">Bambang</t>
   </si>
   <si>
-    <t xml:space="preserve">Not mentioned in the Indian Mahabharata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Arjuna.</t>
+    <t xml:space="preserve">He is the son of </t>
   </si>
   <si>
     <t xml:space="preserve">Dresanala</t>
   </si>
   <si>
+    <t xml:space="preserve">Mustikawati:x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing pages!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">242-245 (Vol. IX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1138-1139</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rungsit</t>
   </si>
   <si>
@@ -4337,6 +4383,18 @@
   </si>
   <si>
     <t xml:space="preserve">A cart pulled by 7 horses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenga_Jayengkaton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to see demons and other invisible creatures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watu_Tempuru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to fight demons and other invisible creatures. </t>
   </si>
   <si>
     <t xml:space="preserve">anoman</t>
@@ -4377,7 +4435,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4511,12 +4569,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -4571,7 +4623,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4680,15 +4732,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4772,44 +4828,44 @@
   <dimension ref="A1:AC148"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A137" activeCellId="0" sqref="A137"/>
-      <selection pane="bottomRight" activeCell="X140" activeCellId="0" sqref="X140"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.6530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.1224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.6530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="33.6938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="61.234693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="99.030612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="34.4489795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="26.780612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="38.1224489795918"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="58.75"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="29.0510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="23.6530612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="46.7602040816327"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="40.5"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="57.8826530612245"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="55.0765306122449"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="52.484693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.515306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.515306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="34.7755102040816"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="63.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="102.377551020408"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="41.2551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="26.0255102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="35.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.6479591836735"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="60.6938775510204"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="24.6224489795918"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="16.4132653061224"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="22.3571428571429"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="29.9132653061224"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="24.515306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="48.3826530612245"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="41.7959183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="59.8265306122449"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="56.9132653061225"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="54.2142857142857"/>
     <col collapsed="false" hidden="false" max="1023" min="30" style="1" width="5.83163265306122"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="5.83163265306122"/>
   </cols>
@@ -12519,7 +12575,7 @@
       <c r="F139" s="1" t="s">
         <v>1182</v>
       </c>
-      <c r="G139" s="27" t="s">
+      <c r="G139" s="10" t="s">
         <v>1183</v>
       </c>
       <c r="H139" s="1" t="s">
@@ -12534,12 +12590,13 @@
       <c r="K139" s="18" t="s">
         <v>1185</v>
       </c>
-      <c r="L139" s="28" t="s">
+      <c r="L139" s="27" t="s">
         <v>1186</v>
       </c>
       <c r="M139" s="5"/>
+      <c r="P139" s="0"/>
       <c r="Q139" s="5"/>
-      <c r="S139" s="28" t="s">
+      <c r="S139" s="27" t="s">
         <v>1187</v>
       </c>
       <c r="T139" s="2" t="s">
@@ -12548,7 +12605,7 @@
       <c r="U139" s="2" t="n">
         <v>261</v>
       </c>
-      <c r="W139" s="28" t="s">
+      <c r="W139" s="27" t="s">
         <v>1189</v>
       </c>
       <c r="X139" s="2" t="s">
@@ -12559,7 +12616,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="s">
+      <c r="A140" s="28" t="s">
         <v>160</v>
       </c>
       <c r="B140" s="5"/>
@@ -12578,21 +12635,35 @@
       <c r="G140" s="1" t="s">
         <v>1192</v>
       </c>
-      <c r="H140" s="0"/>
+      <c r="H140" s="0" t="s">
+        <v>1193</v>
+      </c>
       <c r="I140" s="5"/>
       <c r="J140" s="5"/>
       <c r="K140" s="0"/>
+      <c r="L140" s="0"/>
       <c r="M140" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="P140" s="1" t="s">
+        <v>1194</v>
+      </c>
       <c r="Q140" s="5"/>
       <c r="S140" s="0"/>
+      <c r="T140" s="2" t="n">
+        <v>582</v>
+      </c>
+      <c r="U140" s="0"/>
+      <c r="W140" s="0"/>
+      <c r="X140" s="2" t="s">
+        <v>1195</v>
+      </c>
       <c r="Y140" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
+      <c r="A141" s="6" t="s">
         <v>331</v>
       </c>
       <c r="B141" s="1" t="s">
@@ -12602,33 +12673,48 @@
         <v>27</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
       <c r="H141" s="0"/>
       <c r="I141" s="1" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="J141" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K141" s="0"/>
+      <c r="L141" s="1" t="s">
+        <v>1199</v>
+      </c>
       <c r="Q141" s="5"/>
+      <c r="T141" s="29" t="s">
+        <v>1200</v>
+      </c>
+      <c r="U141" s="2" t="n">
+        <v>263</v>
+      </c>
+      <c r="W141" s="2" t="s">
+        <v>1201</v>
+      </c>
+      <c r="X141" s="2" t="s">
+        <v>1202</v>
+      </c>
       <c r="Y141" s="1" t="s">
-        <v>1197</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>1198</v>
+        <v>1204</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>92</v>
@@ -12640,23 +12726,23 @@
         <v>29</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>1199</v>
+        <v>1205</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>1200</v>
+        <v>1206</v>
       </c>
       <c r="H142" s="0"/>
       <c r="K142" s="0"/>
       <c r="Q142" s="1" t="s">
-        <v>1201</v>
+        <v>1207</v>
       </c>
       <c r="Y142" s="1" t="s">
-        <v>1202</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>1203</v>
+        <v>1209</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>92</v>
@@ -12668,13 +12754,13 @@
         <v>65</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>1204</v>
+        <v>1210</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>1205</v>
+        <v>1211</v>
       </c>
       <c r="K143" s="0"/>
       <c r="Q143" s="5"/>
@@ -12684,7 +12770,7 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>1206</v>
+        <v>1212</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>92</v>
@@ -12696,13 +12782,13 @@
         <v>65</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>1207</v>
+        <v>1213</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>1208</v>
+        <v>1214</v>
       </c>
       <c r="K144" s="0"/>
       <c r="Q144" s="5"/>
@@ -12712,7 +12798,7 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>1209</v>
+        <v>1215</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>92</v>
@@ -12724,14 +12810,14 @@
         <v>29</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>1210</v>
+        <v>1216</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>1211</v>
+        <v>1217</v>
       </c>
       <c r="K145" s="0"/>
       <c r="Q145" s="1" t="s">
-        <v>1212</v>
+        <v>1218</v>
       </c>
       <c r="Y145" s="1" t="s">
         <v>62</v>
@@ -12739,7 +12825,7 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>1213</v>
+        <v>1219</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>27</v>
@@ -12751,10 +12837,10 @@
         <v>29</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1214</v>
+        <v>1220</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>1215</v>
+        <v>1221</v>
       </c>
       <c r="K146" s="0"/>
       <c r="Y146" s="1" t="s">
@@ -12763,22 +12849,22 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>1216</v>
+        <v>1222</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>1217</v>
+        <v>1223</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>1218</v>
+        <v>1224</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>1219</v>
+        <v>1225</v>
       </c>
       <c r="K147" s="0"/>
       <c r="Y147" s="5" t="s">
@@ -12787,7 +12873,7 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>1220</v>
+        <v>1226</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>376</v>
@@ -12802,10 +12888,10 @@
         <v>180</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>1221</v>
+        <v>1227</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>1222</v>
+        <v>1228</v>
       </c>
       <c r="Y148" s="1" t="s">
         <v>62</v>
@@ -12835,48 +12921,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="16.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1367</v>
+        <v>1377</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1368</v>
+        <v>1378</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1369</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1370</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1371</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1372</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1373</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1374</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1375</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12886,7 +12972,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>1376</v>
+        <v>1386</v>
       </c>
     </row>
   </sheetData>
@@ -12917,29 +13003,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="45.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="93.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="104.107142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="76.6734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="46.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="76.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="97.0867346938775"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="107.668367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="79.265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="79.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>1223</v>
+        <v>1229</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1224</v>
+        <v>1230</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1225</v>
+        <v>1231</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>1226</v>
+        <v>1232</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>24</v>
@@ -12963,10 +13049,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>1212</v>
+        <v>1218</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1209</v>
+        <v>1215</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12978,7 +13064,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>1227</v>
+        <v>1233</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>53</v>
@@ -12991,7 +13077,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>1228</v>
+        <v>1234</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>53</v>
@@ -13006,7 +13092,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>1229</v>
+        <v>1235</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>316</v>
@@ -13036,10 +13122,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>1201</v>
+        <v>1207</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1198</v>
+        <v>1204</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -13061,7 +13147,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="H9" s="3" t="s">
-        <v>1230</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13078,12 +13164,12 @@
         <v>62</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>1231</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>1232</v>
+        <v>1238</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>151</v>
@@ -13109,7 +13195,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>1233</v>
+        <v>1239</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>235</v>
@@ -13121,7 +13207,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>1234</v>
+        <v>1240</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>108</v>
@@ -13134,10 +13220,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>1235</v>
+        <v>1241</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1236</v>
+        <v>1242</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -13147,14 +13233,14 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>1237</v>
+        <v>1243</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="3" t="s">
-        <v>1238</v>
+        <v>1244</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>62</v>
@@ -13162,10 +13248,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>1239</v>
+        <v>1245</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1240</v>
+        <v>1246</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -13175,7 +13261,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>1241</v>
+        <v>1247</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>483</v>
@@ -13186,14 +13272,14 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>1242</v>
+        <v>1248</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3" t="s">
-        <v>1243</v>
+        <v>1249</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>62</v>
@@ -13208,7 +13294,7 @@
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1" t="s">
-        <v>1244</v>
+        <v>1250</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>62</v>
@@ -13255,22 +13341,22 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>1245</v>
+        <v>1251</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="1" t="s">
-        <v>1246</v>
+        <v>1252</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29" t="s">
-        <v>1247</v>
+      <c r="A25" s="30" t="s">
+        <v>1253</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>34</v>
@@ -13281,7 +13367,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>1248</v>
+        <v>1254</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>747</v>
@@ -13300,7 +13386,7 @@
         <v>111</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>1249</v>
+        <v>1255</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
@@ -13309,7 +13395,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>1250</v>
+        <v>1256</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>375</v>
@@ -13326,7 +13412,7 @@
         <v>112</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>1251</v>
+        <v>1257</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
@@ -13338,7 +13424,7 @@
         <v>1060</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1252</v>
+        <v>1258</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
@@ -13384,10 +13470,10 @@
         <v>922</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1253</v>
+        <v>1259</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>1254</v>
+        <v>1260</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>62</v>
@@ -13395,7 +13481,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>1255</v>
+        <v>1261</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>34</v>
@@ -13428,12 +13514,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="32.9387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1256</v>
+        <v>1262</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>7</v>
@@ -13447,33 +13533,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1257</v>
+        <v>1263</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1258</v>
+        <v>1264</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1259</v>
+        <v>1265</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1260</v>
+        <v>1266</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="5" t="s">
-        <v>1261</v>
+        <v>1267</v>
       </c>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1262</v>
+        <v>1268</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="5" t="s">
-        <v>1263</v>
+        <v>1269</v>
       </c>
       <c r="D4" s="0"/>
     </row>
@@ -13482,19 +13568,19 @@
         <v>514</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1264</v>
+        <v>1270</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1265</v>
+        <v>1271</v>
       </c>
       <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1266</v>
+        <v>1272</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1267</v>
+        <v>1273</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" s="0"/>
@@ -13510,7 +13596,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>1268</v>
+        <v>1274</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -13539,31 +13625,31 @@
         <v>689</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1269</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>1270</v>
+        <v>1276</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1271</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>1272</v>
+        <v>1278</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>1273</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>1274</v>
+        <v>1280</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>1275</v>
+        <v>1281</v>
       </c>
     </row>
   </sheetData>
@@ -13590,16 +13676,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="50.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="B1" s="5" t="s">
-        <v>1276</v>
+        <v>1282</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1277</v>
+        <v>1283</v>
       </c>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
@@ -13612,13 +13698,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1278</v>
+        <v>1284</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1278</v>
+        <v>1284</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1279</v>
+        <v>1285</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
@@ -13628,7 +13714,7 @@
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="W2" s="5" t="s">
-        <v>1278</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13657,7 +13743,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1280</v>
+        <v>1286</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0"/>
@@ -13671,7 +13757,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1281</v>
+        <v>1287</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0"/>
@@ -13685,7 +13771,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1282</v>
+        <v>1288</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
@@ -13699,7 +13785,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>1283</v>
+        <v>1289</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
@@ -13708,18 +13794,18 @@
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="J8" s="5" t="s">
-        <v>1284</v>
+        <v>1290</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>1285</v>
+        <v>1291</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>1286</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>1287</v>
+        <v>1293</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
@@ -13728,21 +13814,21 @@
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="J9" s="5" t="s">
-        <v>1288</v>
+        <v>1294</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>1289</v>
+        <v>1295</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>1290</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>1291</v>
+        <v>1297</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1292</v>
+        <v>1298</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
@@ -13750,18 +13836,18 @@
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="J10" s="5" t="s">
-        <v>1293</v>
+        <v>1299</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>1294</v>
+        <v>1300</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>1295</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>1296</v>
+        <v>1302</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -13770,18 +13856,18 @@
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="J11" s="5" t="s">
-        <v>1297</v>
+        <v>1303</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>1298</v>
+        <v>1304</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>1299</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>1300</v>
+        <v>1306</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
@@ -13790,21 +13876,21 @@
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="J12" s="5" t="s">
-        <v>1301</v>
+        <v>1307</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>1302</v>
+        <v>1308</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>1303</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>1304</v>
+        <v>1310</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1305</v>
+        <v>1311</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
@@ -13812,21 +13898,21 @@
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="J13" s="5" t="s">
-        <v>1306</v>
+        <v>1312</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>1307</v>
+        <v>1313</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>1308</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>1309</v>
+        <v>1315</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1310</v>
+        <v>1316</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
@@ -13835,10 +13921,10 @@
       <c r="G14" s="0"/>
       <c r="J14" s="0"/>
       <c r="L14" s="5" t="s">
-        <v>1311</v>
+        <v>1317</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>1312</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13855,7 +13941,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>1313</v>
+        <v>1319</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -13864,13 +13950,13 @@
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="J16" s="5" t="s">
-        <v>1314</v>
+        <v>1320</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>1315</v>
+        <v>1321</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>1316</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13882,18 +13968,18 @@
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="J17" s="5" t="s">
-        <v>1317</v>
+        <v>1323</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>1318</v>
+        <v>1324</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>1319</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>1320</v>
+        <v>1326</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -13902,15 +13988,15 @@
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="J18" s="5" t="s">
-        <v>1321</v>
+        <v>1327</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>1322</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>1323</v>
+        <v>1329</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
@@ -13919,7 +14005,7 @@
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
       <c r="J19" s="5" t="s">
-        <v>1324</v>
+        <v>1330</v>
       </c>
       <c r="L19" s="0"/>
     </row>
@@ -13935,7 +14021,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>1325</v>
+        <v>1331</v>
       </c>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -13957,7 +14043,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>1326</v>
+        <v>1332</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -13969,10 +14055,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>1327</v>
+        <v>1333</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1328</v>
+        <v>1334</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
@@ -13980,7 +14066,7 @@
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
       <c r="L24" s="5" t="s">
-        <v>1329</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13992,15 +14078,15 @@
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
       <c r="L25" s="5" t="s">
-        <v>1330</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>1331</v>
+        <v>1337</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1332</v>
+        <v>1338</v>
       </c>
       <c r="C26" s="0"/>
       <c r="D26" s="0"/>
@@ -14008,7 +14094,7 @@
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
       <c r="L26" s="5" t="s">
-        <v>1333</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14020,12 +14106,12 @@
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="L27" s="5" t="s">
-        <v>1334</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>1335</v>
+        <v>1341</v>
       </c>
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
@@ -14034,7 +14120,7 @@
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
       <c r="L28" s="5" t="s">
-        <v>1336</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14056,7 +14142,7 @@
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
       <c r="L30" s="5" t="s">
-        <v>1337</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14068,7 +14154,7 @@
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="L31" s="5" t="s">
-        <v>1338</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14080,7 +14166,7 @@
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
       <c r="L32" s="5" t="s">
-        <v>1339</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14092,7 +14178,7 @@
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="L33" s="5" t="s">
-        <v>1340</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14104,38 +14190,38 @@
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>
       <c r="L34" s="5" t="s">
-        <v>1341</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>1280</v>
+        <v>1286</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1282</v>
+        <v>1288</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1281</v>
+        <v>1287</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1296</v>
+        <v>1302</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1342</v>
+        <v>1348</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1331</v>
+        <v>1337</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>1343</v>
+        <v>1349</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>1344</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L36" s="5" t="s">
-        <v>1345</v>
+        <v>1351</v>
       </c>
     </row>
   </sheetData>
@@ -14162,7 +14248,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="12.0969387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14170,15 +14256,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1346</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1347</v>
+        <v>1353</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1348</v>
+        <v>1354</v>
       </c>
     </row>
   </sheetData>
@@ -14197,15 +14283,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="12.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14213,10 +14299,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1349</v>
+        <v>1355</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1350</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14224,7 +14310,7 @@
         <v>613</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1351</v>
+        <v>1357</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>609</v>
@@ -14232,10 +14318,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1352</v>
+        <v>1358</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1353</v>
+        <v>1359</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>196</v>
@@ -14243,10 +14329,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1354</v>
+        <v>1360</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1355</v>
+        <v>1361</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>196</v>
@@ -14254,18 +14340,18 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1356</v>
+        <v>1362</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1358</v>
+        <v>1364</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1359</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14273,7 +14359,7 @@
         <v>776</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1360</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14281,7 +14367,7 @@
         <v>806</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1361</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14289,7 +14375,7 @@
         <v>964</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1362</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14297,7 +14383,7 @@
         <v>1025</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1363</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14305,7 +14391,7 @@
         <v>1046</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1364</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14313,7 +14399,7 @@
         <v>1098</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1365</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14321,7 +14407,23 @@
         <v>1118</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1366</v>
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1376</v>
       </c>
     </row>
   </sheetData>
@@ -14348,7 +14450,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="16.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14374,7 +14476,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="16.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14400,7 +14502,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="16.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
preliminary version, no images no explanation yet
</commit_message>
<xml_diff>
--- a/input/characters.xlsx
+++ b/input/characters.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="1387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2283" uniqueCount="1413">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -965,7 +965,7 @@
     <t xml:space="preserve">Samba, Gunadewa, Partadewa,Titisari,Saranadewa, Setyaka, Siti_Sendar, Saketi</t>
   </si>
   <si>
-    <t xml:space="preserve">Hagnyanawati: Watubaji</t>
+    <t xml:space="preserve">Hagnyawati: Watubaji</t>
   </si>
   <si>
     <t xml:space="preserve">Aji Pangasonabumi, Puska Wijayamulya, Garuda Wilumna, Pusaka Wijayakusuma</t>
@@ -3787,7 +3787,7 @@
     <t xml:space="preserve">Vibisana is the younger brother of Ravana. In the Indian Ramayana, he is a giant, not a human. </t>
   </si>
   <si>
-    <t xml:space="preserve">He is the younger brother of [Desamuka]. He is the only one who has born with human face (this is different in India). Before [Rama]'s attack to Alengka, he defected to [Rama]'s side, providing vital information on the weaknesses of Alengka's army. His role is controversial – is he noble since he defected? Or should he have stayed to fight for his land, as [Kumbakarna] did? There are multiple opinions on this, which are explored differently by various dalang. After [Desamuka] was killed, Wibisana became king of Alengka, which was thereafter known as Singgelapura. He then received [Rama]'s advice on kingship, in the form of the Hastabrata, a philosophical treaty on statehood. After the Ramayana, he was known as Begawan Kunta Wibisana. He eventually abdicated in favor of his son [Dentawilukrama], and then achieved perfect death.</t>
+    <t xml:space="preserve">He is the younger brother of [Desamuka]. He is the only one who has born with human face (this is different in India). Before [Rama]'s attack to Alengka, he defected to [Rama]'s side, providing vital information on the weaknesses of Alengka's army. His role is controversial and his defection makes some people question the nobility of his character. Should he have stayed to fight for his land, as [Kumbakarna] did? There are multiple opinions on this, which are explored differently by various dalang. After [Desamuka] was killed, Wibisana became king of Alengka, which was thereafter known as Singgelapura. He then received [Rama]'s advice on kingship, in the form of the Hastabrata, a philosophical treaty on statehood. After the Ramayana, he was known as Begawan Kunta Wibisana. He eventually abdicated in favor of his son [Dentawilukrama], and then achieved perfect death.</t>
   </si>
   <si>
     <t xml:space="preserve">Kontawibisana, Kunta_Wibisana, Gunawan_Wibisana</t>
@@ -3881,31 +3881,55 @@
     <t xml:space="preserve">Wisnu</t>
   </si>
   <si>
-    <t xml:space="preserve">Vishnu is known as Preserver. He is the brother of Uma and brother-in-law of Lord Shiva. He is famous for his Dasavatar (10 incarnations)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also known as Narayana. Son of Uma and Guru. The following are considered incarnations of him: Srimaharaja Kanwa, Resi Wisnungkara, Prabu Arjunasasrabahu, Sri Ramawijaya, Sri Batara Kresna . Prabu Airlangga, Prabu Jayabaya, Prabu Anglingdarma Prabu Ken Arok, Prabu Kertawardhana.</t>
+    <t xml:space="preserve">Vishnu is known as The Preserver. He is the brother of Uma and brother-in-law of Lord Shiva. He is famous for his Dasavatar (10 incarnations).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the wayang world, Batara Wisnu is best known for his incarnations: [Rama], [Arjuna_Sasrabahu], [Kresna] and [Arjuna]. [Kresna] is said to be Wisnu's incarnation as thinker and [Arjuna] is Wisnu's incarnation as agent. There are many other stories in the Mahabharata about smaller incarnations of Wisnu into animals or people in order to rectify a misdeed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batara_Suman, Batara_Ari, Batara_Narayana, Batara_Kesawa, Kalasekti, Abhuta, Asiyuta, Cakrawati, Hari, Haus, Idopati, Jaggernata, Napila, Pandarik_Aksa, Purusotama, Purwaya, Wiratapura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri_Sekar: Srigata, Srinada, Srinadi; Sri_Pujayanti: Heruyana, Isawa, Bisawa, Isnapurna, Madura, Madudewa, Madusasana, Dewi_Srihunon, Sewi_Srihuni, Pujarta, Panonbuja, Sarwedi;Pertiwi:x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utarasagara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cakra, Cangkok_Wijayakusuma</t>
   </si>
   <si>
     <t xml:space="preserve">_Tiger</t>
   </si>
   <si>
+    <t xml:space="preserve">594-602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">247-252 (Vol. IX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">208-213</t>
+  </si>
+  <si>
     <t xml:space="preserve">No wisnu</t>
   </si>
   <si>
     <t xml:space="preserve">Wulan_Drema</t>
   </si>
   <si>
-    <t xml:space="preserve">Wulan Derma and Dermi (female) are sons of Batara Darma. //kena kutukan incarnasi, masuk ke tubuh salah. Ulan dermi masuk ke Hagnyawati dan Ulan Derma ke tubuhnya Samba. //Harusnya ke Bomanarakasura, maka selingkuhan.</t>
+    <t xml:space="preserve">Wulan Drema and [Wulan_Dremi] are the offspring of Batara [Darma]. They both decide to incarnate as humans and become lovers. {Wulan _Dremi] incarnates into [Hagnyawati] and Wulan Drema into [Samba]. This was either a mistake or a result of a curse since [Hagnyawati] was meant to marry to [Bomanarakasura], [Samba]'s brother. They committed adultery and [Bomanarakasura] became aware of this. He killed [Samba], but [Kresna] brought him back to life. [Kresna] was privy to the fact of [Samba] and [Hagnyawati] were incarnations of Wuland Drema] and [Wulan_Dremi]. Eventually, [Kresna] killed [Samba] and gave his blessing to the marriage of [Hagnyawati] and [Samba].  </t>
   </si>
   <si>
     <t xml:space="preserve">Ulanderma</t>
   </si>
   <si>
+    <t xml:space="preserve">223 (Vol. IV)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wulan_Dremi</t>
   </si>
   <si>
-    <t xml:space="preserve">Wulan Derma (male) and Dermi (female) are born to Batara Darma.</t>
+    <t xml:space="preserve">Wulan [Drema] and Wulan Dremi are the offspring of Batara [Darma]. They both decide to incarnate as humans and become lovers. Wulan Dremi incarnates into [Hagnyawati] and [Wulan_Drema] into [Samba]. This was either a mistake or a result of a curse since [Hagnyawati] was meant to marry to [Bomanarakasura], [Samba]'s brother. They committed adultery and [Bomanarakasura] became aware of this. He killed [Samba], but [Kresna] brought him back to life. [Kresna] was privy to the fact of [Samba] and [Hagnyawati] were incarnations of [Wulan_Drema] and Wulan Dremi. Eventually, [Kresna] killed [Samba] and gave his blessing to the marriage of [Hagnyawati] and [Samba].  </t>
   </si>
   <si>
     <t xml:space="preserve">Ulandermi</t>
@@ -3914,22 +3938,61 @@
     <t xml:space="preserve">Yamadipati</t>
   </si>
   <si>
-    <t xml:space="preserve">Check! Definitely in Indian version.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Yamadipati and Senggani. His wife (Mumpuni) runs away with Bambang Nagatmala (Hyang Antaboga and Dewi Suprepti). His anger makes him half giant.</t>
+    <t xml:space="preserve">Yama is the lord of death.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He is the god of death, responsible for plucking the souls of mortals when their time comes. He has the head of an ogre. He was married to Dewi [Mumpuni], but then she left him and married Batara [Nagatamala]. He once fought [Desamuka], an event that almost triggered the end of the world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petraraja, Yama_Kingkarapati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mumpuni:x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argadumilah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaladenda</t>
   </si>
   <si>
     <t xml:space="preserve">_Guard</t>
   </si>
   <si>
+    <t xml:space="preserve">Bengis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">278-282 (Vol. IX)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yamawidura</t>
   </si>
   <si>
-    <t xml:space="preserve">Vidura is the prime minister in the court of Hastinapura. He is born to Veda Vyasa and one of the maid-servants in the Kuru. He is viewed as a wise man who provides strong support to the Pandavas for the righteousness although he is often placed in a tough spot due to his royal allegiance to the Kuru house where the Kauravas reside and to his sense of consciousness when he witnesses many instances of unfair treatment towards the Pandavas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son of Abyasa and Datri. His half brother are Pandu and Drestarasta. He marries Dewi Pamarini [daughter of Praby Dipacandra] has two sons: Sanjaya dan Yuyutsuh. // satu ayah dengan Pandu dan Destrarastra</t>
+    <t xml:space="preserve">Vidura was the prime minister in the court of Hastinapura. He was born to Veda Vyasa and one of the maid-servants in the Kuru. He was viewed as a wise man who provided strong support to the Pandavas although he was often placed in a tough spot due to his royal allegiance to the Kuru house (where the Kauravas resided) and to his sense of consciousness when he witnessesed many instances of unfair treatment towards the Pandavas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He was well respected by both the Pandawa and the Korawa. He was an avatar of Batara [Darma]. As his brothers, he was born disfigured. In his case, one of his legs was shorter than the other. He tried to prevent the Pandawas from engaging in the game of dice with the Kurawas. He followed the Pandawa into the forest for the first part of their exile, but [Abiyasa] eventually convinced him to return to Astina. He continuously tried to talk [Duryudana] out of engaging in outright war with the Pandawa. He died with [Kunti], [Drestarastra] and [Gendari], at the end of the Baratayuda war. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padmarini:Sanjaya, Yuyutsuh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panukma, Runcit, Buncit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">578-580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160-161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">282-286 (Vol. IX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11466-1147</t>
   </si>
   <si>
     <t xml:space="preserve">Yuda_Kothi</t>
@@ -3938,19 +4001,34 @@
     <t xml:space="preserve">Arya</t>
   </si>
   <si>
-    <t xml:space="preserve">Narada in Hindu mythology is not mentioned as having a vehicle. He is known as trilokasanjaari (the traveller of the three world (Heaven, Earth and the Underworld) as he is able to go to any of these three places that he will. He is known as the son of Brahma the creator and ardent devotee of Vishnu the Preserver)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An elephant-shaped ogre that works for Nagaprasanta. After Baladewa kills Nagraprasanta, Yudakothi becomes a transport for Narada</t>
+    <t xml:space="preserve">Narada in Hindu mythology is not known to have a vehicle. He was known as trilokasanjaari (the traveller of the three worlds: Heaven, Earth and the Underworld) as he was able to go to any of these places at will. He was known as the son of Brahma and ardent devotee of Vishnu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An elephant-shaped ogre that works for [Nagaprasanta]. After [Baladewa] killed [Nagraprasanta], [Yudakothi] became the transport of Narada. No entries for this character were found in any of the consulted encyclopedias.</t>
   </si>
   <si>
     <t xml:space="preserve">Yudhistira</t>
   </si>
   <si>
-    <t xml:space="preserve">Mrentani kingdom. saudara tua dari Arya Dananjaya, Arya Dandunwacana, jim Nakula, dan jim Sadewa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhandhanwacana, Dananjaya, Suparta</t>
+    <t xml:space="preserve">He was the ruler of the invisible kingdom of Mretani. He was defeated by the Pandawa and came to inhabit the body of [Puntadewa], who took Yudistira's name and kingdom. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhandhanwacana, Dananjaya, Suparta, Sapujagad, Sapulebu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahina: Ratri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mretani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">619-622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-294 (Vol. IX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1152-1153</t>
   </si>
   <si>
     <t xml:space="preserve">Diguise</t>
@@ -4435,7 +4513,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4580,6 +4658,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4623,7 +4708,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4744,6 +4829,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4828,44 +4917,44 @@
   <dimension ref="A1:AC148"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C134" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S3" activeCellId="0" sqref="S3"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A134" activeCellId="0" sqref="A134"/>
+      <selection pane="bottomRight" activeCell="G139" activeCellId="0" sqref="G139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.0255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.515306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.7448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.515306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="34.7755102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="63.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="102.377551020408"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="41.2551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="26.0255102040816"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="35.530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.6479591836735"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="60.6938775510204"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="24.6224489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="16.4132653061224"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="22.3571428571429"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="29.9132653061224"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="24.515306122449"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="48.3826530612245"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="41.7959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="59.8265306122449"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="56.9132653061225"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="54.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.8520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.4489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.2142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.7040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.3622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="33.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.7040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="34.4489795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="36.5"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="66.5255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="107.668367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.3061224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="33.9081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="27.2142857142857"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="37.3673469387755"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="29.0510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="41.3622448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="63.8265306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="25.7040816326531"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="23.3265306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="25.7040816326531"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="43.8469387755102"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="62.8520408163265"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="59.8265306122449"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="56.9132653061225"/>
     <col collapsed="false" hidden="false" max="1023" min="30" style="1" width="5.83163265306122"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="5.83163265306122"/>
   </cols>
@@ -12530,6 +12619,7 @@
         <v>1175</v>
       </c>
       <c r="M138" s="5"/>
+      <c r="N138" s="0"/>
       <c r="P138" s="1" t="s">
         <v>1176</v>
       </c>
@@ -12594,6 +12684,7 @@
         <v>1186</v>
       </c>
       <c r="M139" s="5"/>
+      <c r="N139" s="0"/>
       <c r="P139" s="0"/>
       <c r="Q139" s="5"/>
       <c r="S139" s="27" t="s">
@@ -12605,6 +12696,7 @@
       <c r="U139" s="2" t="n">
         <v>261</v>
       </c>
+      <c r="V139" s="0"/>
       <c r="W139" s="27" t="s">
         <v>1189</v>
       </c>
@@ -12645,6 +12737,7 @@
       <c r="M140" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="N140" s="0"/>
       <c r="P140" s="1" t="s">
         <v>1194</v>
       </c>
@@ -12654,6 +12747,7 @@
         <v>582</v>
       </c>
       <c r="U140" s="0"/>
+      <c r="V140" s="0"/>
       <c r="W140" s="0"/>
       <c r="X140" s="2" t="s">
         <v>1195</v>
@@ -12695,13 +12789,17 @@
       <c r="L141" s="1" t="s">
         <v>1199</v>
       </c>
+      <c r="N141" s="0"/>
+      <c r="P141" s="0"/>
       <c r="Q141" s="5"/>
+      <c r="S141" s="0"/>
       <c r="T141" s="29" t="s">
         <v>1200</v>
       </c>
       <c r="U141" s="2" t="n">
         <v>263</v>
       </c>
+      <c r="V141" s="0"/>
       <c r="W141" s="2" t="s">
         <v>1201</v>
       </c>
@@ -12712,8 +12810,8 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="s">
+    <row r="142" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="6" t="s">
         <v>1204</v>
       </c>
       <c r="C142" s="1" t="s">
@@ -12731,18 +12829,49 @@
       <c r="G142" s="1" t="s">
         <v>1206</v>
       </c>
-      <c r="H142" s="0"/>
+      <c r="H142" s="0" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I142" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="J142" s="0" t="s">
+        <v>240</v>
+      </c>
       <c r="K142" s="0"/>
+      <c r="L142" s="0" t="s">
+        <v>1208</v>
+      </c>
+      <c r="N142" s="0" t="s">
+        <v>1209</v>
+      </c>
+      <c r="P142" s="0" t="s">
+        <v>1210</v>
+      </c>
       <c r="Q142" s="1" t="s">
-        <v>1207</v>
+        <v>1211</v>
+      </c>
+      <c r="S142" s="0"/>
+      <c r="T142" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="U142" s="2" t="n">
+        <v>265</v>
+      </c>
+      <c r="V142" s="0"/>
+      <c r="W142" s="0" t="s">
+        <v>1213</v>
+      </c>
+      <c r="X142" s="2" t="s">
+        <v>1214</v>
       </c>
       <c r="Y142" s="1" t="s">
-        <v>1208</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
-        <v>1209</v>
+      <c r="A143" s="6" t="s">
+        <v>1216</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>92</v>
@@ -12756,21 +12885,36 @@
       <c r="F143" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="G143" s="1" t="s">
-        <v>1210</v>
+      <c r="G143" s="30" t="s">
+        <v>1217</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>1211</v>
-      </c>
+        <v>1218</v>
+      </c>
+      <c r="I143" s="0"/>
+      <c r="J143" s="0"/>
       <c r="K143" s="0"/>
+      <c r="L143" s="0"/>
+      <c r="N143" s="0"/>
+      <c r="P143" s="0"/>
       <c r="Q143" s="5"/>
+      <c r="S143" s="0"/>
+      <c r="T143" s="0"/>
+      <c r="U143" s="0"/>
+      <c r="V143" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="W143" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="X143" s="0"/>
       <c r="Y143" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="s">
-        <v>1212</v>
+      <c r="A144" s="6" t="s">
+        <v>1220</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>92</v>
@@ -12784,21 +12928,34 @@
       <c r="F144" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="G144" s="1" t="s">
-        <v>1213</v>
+      <c r="G144" s="30" t="s">
+        <v>1221</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>1214</v>
-      </c>
+        <v>1222</v>
+      </c>
+      <c r="I144" s="0"/>
+      <c r="J144" s="0"/>
       <c r="K144" s="0"/>
+      <c r="L144" s="0"/>
+      <c r="N144" s="0"/>
+      <c r="P144" s="0"/>
       <c r="Q144" s="5"/>
+      <c r="S144" s="0"/>
+      <c r="T144" s="0"/>
+      <c r="U144" s="0"/>
+      <c r="V144" s="0"/>
+      <c r="W144" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="X144" s="0"/>
       <c r="Y144" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="s">
-        <v>1215</v>
+      <c r="A145" s="6" t="s">
+        <v>1223</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>92</v>
@@ -12810,22 +12967,56 @@
         <v>29</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>1216</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>1217</v>
+        <v>1224</v>
+      </c>
+      <c r="G145" s="10" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>1114</v>
       </c>
       <c r="K145" s="0"/>
+      <c r="L145" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="N145" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="P145" s="1" t="s">
+        <v>1229</v>
+      </c>
       <c r="Q145" s="1" t="s">
-        <v>1218</v>
+        <v>1230</v>
+      </c>
+      <c r="S145" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="T145" s="2" t="n">
+        <v>617</v>
+      </c>
+      <c r="U145" s="2" t="n">
+        <v>269</v>
+      </c>
+      <c r="V145" s="0"/>
+      <c r="W145" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="X145" s="2" t="s">
+        <v>466</v>
       </c>
       <c r="Y145" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
-        <v>1219</v>
+      <c r="A146" s="6" t="s">
+        <v>1233</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>27</v>
@@ -12837,43 +13028,80 @@
         <v>29</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1220</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>1221</v>
+        <v>1234</v>
+      </c>
+      <c r="G146" s="10" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="K146" s="0"/>
+      <c r="L146" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="N146" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="P146" s="0"/>
+      <c r="S146" s="0" t="s">
+        <v>1238</v>
+      </c>
+      <c r="T146" s="0" t="s">
+        <v>1239</v>
+      </c>
+      <c r="U146" s="2" t="n">
+        <v>270</v>
+      </c>
+      <c r="V146" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="W146" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="X146" s="2" t="s">
+        <v>1242</v>
+      </c>
       <c r="Y146" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="s">
-        <v>1222</v>
+      <c r="A147" s="6" t="s">
+        <v>1243</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>1223</v>
+        <v>1244</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>1224</v>
+        <v>1245</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>1225</v>
+        <v>1246</v>
       </c>
       <c r="K147" s="0"/>
+      <c r="L147" s="0"/>
+      <c r="N147" s="0"/>
+      <c r="T147" s="0"/>
+      <c r="U147" s="0"/>
+      <c r="W147" s="0"/>
+      <c r="X147" s="0"/>
       <c r="Y147" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="s">
-        <v>1226</v>
+      <c r="A148" s="6" t="s">
+        <v>1247</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>376</v>
@@ -12887,11 +13115,29 @@
       <c r="F148" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G148" s="1" t="s">
-        <v>1227</v>
+      <c r="G148" s="10" t="s">
+        <v>1248</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>1228</v>
+        <v>1249</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="N148" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="T148" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="U148" s="2" t="n">
+        <v>271</v>
+      </c>
+      <c r="W148" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="X148" s="2" t="s">
+        <v>1254</v>
       </c>
       <c r="Y148" s="1" t="s">
         <v>62</v>
@@ -12921,48 +13167,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="18.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1377</v>
+        <v>1403</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1378</v>
+        <v>1404</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1379</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1380</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1381</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1382</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1383</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1384</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1385</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12972,7 +13218,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>1386</v>
+        <v>1412</v>
       </c>
     </row>
   </sheetData>
@@ -13003,29 +13249,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="97.0867346938775"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="107.668367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="79.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="79.265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="49.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="102.163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="113.392857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="49.8928571428572"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="83.3724489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>1229</v>
+        <v>1255</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1230</v>
+        <v>1256</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1231</v>
+        <v>1257</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>1232</v>
+        <v>1258</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>24</v>
@@ -13049,10 +13295,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>1218</v>
+        <v>1230</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1215</v>
+        <v>1223</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -13064,7 +13310,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>1233</v>
+        <v>1259</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>53</v>
@@ -13077,7 +13323,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>1234</v>
+        <v>1260</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>53</v>
@@ -13092,7 +13338,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>1235</v>
+        <v>1261</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>316</v>
@@ -13122,7 +13368,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>1207</v>
+        <v>1211</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1204</v>
@@ -13147,7 +13393,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="H9" s="3" t="s">
-        <v>1236</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13164,12 +13410,12 @@
         <v>62</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>1237</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>1238</v>
+        <v>1264</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>151</v>
@@ -13195,7 +13441,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>1239</v>
+        <v>1265</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>235</v>
@@ -13207,7 +13453,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>1240</v>
+        <v>1266</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>108</v>
@@ -13220,10 +13466,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>1241</v>
+        <v>1267</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1242</v>
+        <v>1268</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -13233,14 +13479,14 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>1243</v>
+        <v>1269</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="3" t="s">
-        <v>1244</v>
+        <v>1270</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>62</v>
@@ -13248,10 +13494,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>1245</v>
+        <v>1271</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1246</v>
+        <v>1272</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -13261,7 +13507,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>1247</v>
+        <v>1273</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>483</v>
@@ -13272,14 +13518,14 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>1248</v>
+        <v>1274</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3" t="s">
-        <v>1249</v>
+        <v>1275</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>62</v>
@@ -13294,7 +13540,7 @@
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1" t="s">
-        <v>1250</v>
+        <v>1276</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>62</v>
@@ -13341,22 +13587,22 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>1251</v>
+        <v>1277</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="1" t="s">
-        <v>1252</v>
+        <v>1278</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
-        <v>1253</v>
+      <c r="A25" s="31" t="s">
+        <v>1279</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>34</v>
@@ -13367,7 +13613,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>1254</v>
+        <v>1280</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>747</v>
@@ -13386,7 +13632,7 @@
         <v>111</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>1255</v>
+        <v>1281</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
@@ -13395,7 +13641,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>1256</v>
+        <v>1282</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>375</v>
@@ -13412,7 +13658,7 @@
         <v>112</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>1257</v>
+        <v>1283</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
@@ -13424,7 +13670,7 @@
         <v>1060</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1258</v>
+        <v>1284</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
@@ -13470,10 +13716,10 @@
         <v>922</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1259</v>
+        <v>1285</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>1260</v>
+        <v>1286</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>62</v>
@@ -13481,7 +13727,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>1261</v>
+        <v>1287</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>34</v>
@@ -13514,12 +13760,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="34.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1262</v>
+        <v>1288</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>7</v>
@@ -13533,33 +13779,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1263</v>
+        <v>1289</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1264</v>
+        <v>1290</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1265</v>
+        <v>1291</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1266</v>
+        <v>1292</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="5" t="s">
-        <v>1267</v>
+        <v>1293</v>
       </c>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1268</v>
+        <v>1294</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="5" t="s">
-        <v>1269</v>
+        <v>1295</v>
       </c>
       <c r="D4" s="0"/>
     </row>
@@ -13568,19 +13814,19 @@
         <v>514</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1270</v>
+        <v>1296</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1271</v>
+        <v>1297</v>
       </c>
       <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1272</v>
+        <v>1298</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1273</v>
+        <v>1299</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" s="0"/>
@@ -13596,7 +13842,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -13625,31 +13871,31 @@
         <v>689</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1275</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>1276</v>
+        <v>1302</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1277</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>1278</v>
+        <v>1304</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>1279</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>1280</v>
+        <v>1306</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>1281</v>
+        <v>1307</v>
       </c>
     </row>
   </sheetData>
@@ -13676,16 +13922,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="53.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="B1" s="5" t="s">
-        <v>1282</v>
+        <v>1308</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1283</v>
+        <v>1309</v>
       </c>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
@@ -13698,13 +13944,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1284</v>
+        <v>1310</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1284</v>
+        <v>1310</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1285</v>
+        <v>1311</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
@@ -13714,7 +13960,7 @@
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="W2" s="5" t="s">
-        <v>1284</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13743,7 +13989,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1286</v>
+        <v>1312</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0"/>
@@ -13757,7 +14003,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1287</v>
+        <v>1313</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0"/>
@@ -13771,7 +14017,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1288</v>
+        <v>1314</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
@@ -13785,7 +14031,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>1289</v>
+        <v>1315</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
@@ -13794,18 +14040,18 @@
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="J8" s="5" t="s">
-        <v>1290</v>
+        <v>1316</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>1291</v>
+        <v>1317</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>1292</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>1293</v>
+        <v>1319</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
@@ -13814,21 +14060,21 @@
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="J9" s="5" t="s">
-        <v>1294</v>
+        <v>1320</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>1295</v>
+        <v>1321</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>1296</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>1297</v>
+        <v>1323</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1298</v>
+        <v>1324</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
@@ -13836,18 +14082,18 @@
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="J10" s="5" t="s">
-        <v>1299</v>
+        <v>1325</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>1300</v>
+        <v>1326</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>1301</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>1302</v>
+        <v>1328</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -13856,18 +14102,18 @@
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="J11" s="5" t="s">
-        <v>1303</v>
+        <v>1329</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>1304</v>
+        <v>1330</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>1305</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>1306</v>
+        <v>1332</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
@@ -13876,21 +14122,21 @@
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="J12" s="5" t="s">
-        <v>1307</v>
+        <v>1333</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>1308</v>
+        <v>1334</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>1309</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>1310</v>
+        <v>1336</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1311</v>
+        <v>1337</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
@@ -13898,21 +14144,21 @@
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="J13" s="5" t="s">
-        <v>1312</v>
+        <v>1338</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>1313</v>
+        <v>1339</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>1314</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>1315</v>
+        <v>1341</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1316</v>
+        <v>1342</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
@@ -13921,10 +14167,10 @@
       <c r="G14" s="0"/>
       <c r="J14" s="0"/>
       <c r="L14" s="5" t="s">
-        <v>1317</v>
+        <v>1343</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>1318</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13941,7 +14187,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>1319</v>
+        <v>1345</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -13950,13 +14196,13 @@
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="J16" s="5" t="s">
-        <v>1320</v>
+        <v>1346</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>1321</v>
+        <v>1347</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>1322</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13968,18 +14214,18 @@
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="J17" s="5" t="s">
-        <v>1323</v>
+        <v>1349</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>1324</v>
+        <v>1350</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>1325</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>1326</v>
+        <v>1352</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -13988,15 +14234,15 @@
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="J18" s="5" t="s">
-        <v>1327</v>
+        <v>1353</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>1328</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>1329</v>
+        <v>1355</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
@@ -14005,7 +14251,7 @@
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
       <c r="J19" s="5" t="s">
-        <v>1330</v>
+        <v>1356</v>
       </c>
       <c r="L19" s="0"/>
     </row>
@@ -14021,7 +14267,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>1331</v>
+        <v>1357</v>
       </c>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -14043,7 +14289,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>1332</v>
+        <v>1358</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -14055,10 +14301,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>1333</v>
+        <v>1359</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1334</v>
+        <v>1360</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
@@ -14066,7 +14312,7 @@
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
       <c r="L24" s="5" t="s">
-        <v>1335</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14078,15 +14324,15 @@
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
       <c r="L25" s="5" t="s">
-        <v>1336</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>1337</v>
+        <v>1363</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1338</v>
+        <v>1364</v>
       </c>
       <c r="C26" s="0"/>
       <c r="D26" s="0"/>
@@ -14094,7 +14340,7 @@
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
       <c r="L26" s="5" t="s">
-        <v>1339</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14106,12 +14352,12 @@
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="L27" s="5" t="s">
-        <v>1340</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>1341</v>
+        <v>1367</v>
       </c>
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
@@ -14120,7 +14366,7 @@
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
       <c r="L28" s="5" t="s">
-        <v>1342</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14142,7 +14388,7 @@
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
       <c r="L30" s="5" t="s">
-        <v>1343</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14154,7 +14400,7 @@
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="L31" s="5" t="s">
-        <v>1344</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14166,7 +14412,7 @@
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
       <c r="L32" s="5" t="s">
-        <v>1345</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14178,7 +14424,7 @@
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="L33" s="5" t="s">
-        <v>1346</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14190,38 +14436,38 @@
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>
       <c r="L34" s="5" t="s">
-        <v>1347</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>1286</v>
+        <v>1312</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1288</v>
+        <v>1314</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1287</v>
+        <v>1313</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1302</v>
+        <v>1328</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1348</v>
+        <v>1374</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1337</v>
+        <v>1363</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>1349</v>
+        <v>1375</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>1350</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L36" s="5" t="s">
-        <v>1351</v>
+        <v>1377</v>
       </c>
     </row>
   </sheetData>
@@ -14248,7 +14494,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="12.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="12.7448979591837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14256,15 +14502,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1352</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1353</v>
+        <v>1379</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1354</v>
+        <v>1380</v>
       </c>
     </row>
   </sheetData>
@@ -14291,7 +14537,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="12.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="12.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14299,10 +14545,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1355</v>
+        <v>1381</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1356</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14310,7 +14556,7 @@
         <v>613</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1357</v>
+        <v>1383</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>609</v>
@@ -14318,10 +14564,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1358</v>
+        <v>1384</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1359</v>
+        <v>1385</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>196</v>
@@ -14329,10 +14575,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1360</v>
+        <v>1386</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1361</v>
+        <v>1387</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>196</v>
@@ -14340,18 +14586,18 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1362</v>
+        <v>1388</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1363</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1364</v>
+        <v>1390</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1365</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14359,7 +14605,7 @@
         <v>776</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1366</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14367,7 +14613,7 @@
         <v>806</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1367</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14375,7 +14621,7 @@
         <v>964</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1368</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14383,7 +14629,7 @@
         <v>1025</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1369</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14391,7 +14637,7 @@
         <v>1046</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1370</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14399,7 +14645,7 @@
         <v>1098</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1371</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14407,23 +14653,23 @@
         <v>1118</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1372</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>1373</v>
+        <v>1399</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1374</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>1375</v>
+        <v>1401</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1376</v>
+        <v>1402</v>
       </c>
     </row>
   </sheetData>
@@ -14450,7 +14696,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="18.25"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14476,7 +14722,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="18.25"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14502,7 +14748,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="17.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="18.25"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
modified malihan names, to ad * at beginning of filename
</commit_message>
<xml_diff>
--- a/input/characters.xlsx
+++ b/input/characters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Canonical" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1443">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -286,7 +286,7 @@
     <t xml:space="preserve">Aji Sepiangin, Aji Pameling, Aji Mundri</t>
   </si>
   <si>
-    <t xml:space="preserve">Amonggati</t>
+    <t xml:space="preserve">*Amonggati</t>
   </si>
   <si>
     <t xml:space="preserve">Naga, Barat, Racut, Cinde</t>
@@ -382,7 +382,7 @@
     <t xml:space="preserve">Pustaka Mustikabumi</t>
   </si>
   <si>
-    <t xml:space="preserve">Bayu_Bajra</t>
+    <t xml:space="preserve">*Bayu_Bajra</t>
   </si>
   <si>
     <t xml:space="preserve">Guntur, Jaka</t>
@@ -481,7 +481,7 @@
     <t xml:space="preserve">Keris Kyai Kalanadah, Panah Pasopati, Panah Sangkali, Panah Cundamanik, Candranila, Sirsha, Dewadata, Baruna, Pulanggeni, Sarotama, Aji Palimunan, Aji Tunggengmaya, Aji Sepiangin, Aji Mayabumi, Aji Pengasih, Aji Asmaragama</t>
   </si>
   <si>
-    <t xml:space="preserve">Godakesa, Lesmana_Murdaka, Suksma_Langgen</t>
+    <t xml:space="preserve">*Godakesa, *Lesmana_Murdaka, *Suksma_Langgen</t>
   </si>
   <si>
     <t xml:space="preserve">Ratmuka</t>
@@ -4043,73 +4043,70 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">-Boar</t>
+    <t xml:space="preserve">*Boar</t>
   </si>
   <si>
     <t xml:space="preserve">Suksma_Langgeng</t>
   </si>
   <si>
-    <t xml:space="preserve">Guard~</t>
+    <t xml:space="preserve">*Guard</t>
   </si>
   <si>
     <t xml:space="preserve">Semar_mBangun_Kayangan</t>
   </si>
   <si>
-    <t xml:space="preserve">Lion-</t>
+    <t xml:space="preserve">*Lion</t>
   </si>
   <si>
     <t xml:space="preserve">Wahyu_Kembar</t>
   </si>
   <si>
-    <t xml:space="preserve">Raksasa*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+Raksasa_One</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~Raksasa_Two</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiger+</t>
+    <t xml:space="preserve">*Raksasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Raksasa_One</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Raksasa_Two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Tiger</t>
   </si>
   <si>
     <t xml:space="preserve">Wahyu_Topeng_Waja</t>
   </si>
   <si>
-    <t xml:space="preserve">Woman</t>
+    <t xml:space="preserve">*Woman</t>
   </si>
   <si>
     <t xml:space="preserve">Citrasena in reality. They want to help the Korawa defeat Pandawa. They are sent by Duryudana to chase Pradapa and Endang Soka. Killed by Nakula and Sadewa in the Sudamala story.</t>
   </si>
   <si>
-    <t xml:space="preserve">*Amonggati</t>
-  </si>
-  <si>
     <t xml:space="preserve">Citrarata in reality. They want to help the Korawa defeat Pandawa. They are sent by Duryudana to chase Pradapa and Endang Soka. Killed by Nakula and Sadewa in the Sudamala story.</t>
   </si>
   <si>
-    <t xml:space="preserve">#Arjuna</t>
+    <t xml:space="preserve">*Arjuna</t>
   </si>
   <si>
     <t xml:space="preserve">Puntadewa_Wisudha</t>
   </si>
   <si>
+    <t xml:space="preserve">*Bagus</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wisanggeni_Lahir</t>
   </si>
   <si>
-    <t xml:space="preserve">~Basudewa</t>
+    <t xml:space="preserve">*Basudewa</t>
   </si>
   <si>
     <t xml:space="preserve">Basudewa_Grogol</t>
   </si>
   <si>
-    <t xml:space="preserve">~Bayu_Bajra</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bandung_Nagasewu</t>
   </si>
   <si>
-    <t xml:space="preserve">~Bimasakti</t>
+    <t xml:space="preserve">*Bimasakti</t>
   </si>
   <si>
     <t xml:space="preserve">Werkudara, Wenang</t>
@@ -4118,52 +4115,52 @@
     <t xml:space="preserve">Prabu_Bimasakti</t>
   </si>
   <si>
-    <t xml:space="preserve">~Brahala</t>
+    <t xml:space="preserve">*Brahala</t>
   </si>
   <si>
     <t xml:space="preserve">The ogre shape that Kresna takes when he is angry.</t>
   </si>
   <si>
-    <t xml:space="preserve">~Werkudara</t>
+    <t xml:space="preserve">*Werkudara</t>
   </si>
   <si>
     <t xml:space="preserve">A pile of weapons in disguise</t>
   </si>
   <si>
-    <t xml:space="preserve">~Gatotkaca</t>
+    <t xml:space="preserve">*Gatotkaca</t>
   </si>
   <si>
     <t xml:space="preserve">Wahyu_Kembar,</t>
   </si>
   <si>
-    <t xml:space="preserve">~Godakesa</t>
+    <t xml:space="preserve">*Godakesa</t>
   </si>
   <si>
     <t xml:space="preserve">Pretends to be the king of Tluki seta in Semar mBagung Kayangan.</t>
   </si>
   <si>
-    <t xml:space="preserve">~Godhayitma</t>
+    <t xml:space="preserve">*Godhayitma</t>
   </si>
   <si>
     <t xml:space="preserve">He is described as the younger brother of Bomanarakasura in lakon Wahyu Topeng Waja. Also meets him in Semar Mantu (Version 2). // He appears in different lakon. He is a spriit of Desamuka.</t>
   </si>
   <si>
-    <t xml:space="preserve">~JakaPupon</t>
+    <t xml:space="preserve">*JakaPupon</t>
   </si>
   <si>
     <t xml:space="preserve">Semar_Mantu_Alternative_Version</t>
   </si>
   <si>
-    <t xml:space="preserve">~Kalanjaya</t>
+    <t xml:space="preserve">*Kalanjaya</t>
   </si>
   <si>
     <t xml:space="preserve">Sudamala</t>
   </si>
   <si>
-    <t xml:space="preserve">~Kalantaka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~Kesawasidhi</t>
+    <t xml:space="preserve">*Kalantaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Kesawasidhi</t>
   </si>
   <si>
     <t xml:space="preserve">Wahyu_Makutharama</t>
@@ -4172,62 +4169,25 @@
     <t xml:space="preserve">A hermitt that lives with Anoman and other hermitts. // Sebenarnya dia amemba Kresna.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">~</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lesmana</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Murdaka</t>
-    </r>
+    <t xml:space="preserve">*Lesmana_Murdaka</t>
   </si>
   <si>
     <t xml:space="preserve">Semar_Boyong_(Wahyu_Katetreman)</t>
   </si>
   <si>
-    <t xml:space="preserve">~Nagabanda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~Nagasewu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~Narada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~Nindyamaya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~RaraTemon</t>
+    <t xml:space="preserve">*Nagabanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Nagasewu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Narada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Nindyamaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*RaraTemon</t>
   </si>
   <si>
     <t xml:space="preserve">SitiSendari, Sri</t>
@@ -4236,19 +4196,19 @@
     <t xml:space="preserve">Semar_Mantu_Alternative_Version, Semar_Mantu</t>
   </si>
   <si>
-    <t xml:space="preserve">~Resi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~Sengkalawati</t>
+    <t xml:space="preserve">*Resi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Sengkalawati</t>
   </si>
   <si>
     <t xml:space="preserve">Wahyu_Cakraningrat</t>
   </si>
   <si>
-    <t xml:space="preserve">~Sinduragen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~Sintawaka</t>
+    <t xml:space="preserve">*Sinduragen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Sintawaka</t>
   </si>
   <si>
     <t xml:space="preserve">RaraIreng</t>
@@ -4257,7 +4217,7 @@
     <t xml:space="preserve">Sintawaka is the male disguise of Rara Ireng.</t>
   </si>
   <si>
-    <t xml:space="preserve">~SuksmaLanggeng</t>
+    <t xml:space="preserve">*SuksmaLanggeng</t>
   </si>
   <si>
     <t xml:space="preserve">Name </t>
@@ -5046,12 +5006,12 @@
   </sheetPr>
   <dimension ref="A1:AC148"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
-      <selection pane="bottomRight" activeCell="G54" activeCellId="0" sqref="G54"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Q16" activeCellId="0" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13302,43 +13262,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1434</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1435</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1436</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13348,7 +13308,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
   </sheetData>
@@ -13369,11 +13329,11 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
       <selection pane="bottomRight" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -13544,7 +13504,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>1272</v>
+        <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>73</v>
@@ -13558,26 +13518,26 @@
         <v>62</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>563</v>
+        <v>1275</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>555</v>
@@ -13607,13 +13567,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>1279</v>
+        <v>117</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
@@ -13622,13 +13582,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>1281</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="D15" s="5" t="s">
         <v>1282</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>1283</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
@@ -13637,16 +13597,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>62</v>
@@ -13654,13 +13614,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>1286</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>1287</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
@@ -13669,20 +13629,20 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>483</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>34</v>
@@ -13691,7 +13651,7 @@
         <v>1262</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>62</v>
@@ -13699,7 +13659,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>332</v>
@@ -13708,7 +13668,7 @@
         <v>1269</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>62</v>
@@ -13716,13 +13676,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>946</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
@@ -13731,13 +13691,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>317</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="3" t="s">
@@ -13746,13 +13706,13 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>312</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="3" t="s">
@@ -13761,16 +13721,16 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>1300</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>1301</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>62</v>
@@ -13778,26 +13738,26 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="31" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>747</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
@@ -13806,13 +13766,13 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>111</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
@@ -13821,20 +13781,20 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>375</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>112</v>
@@ -13849,13 +13809,13 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>1308</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>1309</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>1310</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
@@ -13864,7 +13824,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>380</v>
@@ -13879,13 +13839,13 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>870</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5" t="s">
@@ -13894,7 +13854,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>558</v>
@@ -13907,16 +13867,16 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>1315</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>1316</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>1300</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>1317</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>62</v>
@@ -13924,7 +13884,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>34</v>
@@ -13965,7 +13925,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>7</v>
@@ -13979,33 +13939,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1320</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>1321</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1322</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="5" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="5" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="D4" s="0"/>
     </row>
@@ -14014,19 +13974,19 @@
         <v>514</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>1327</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>1328</v>
       </c>
       <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>1329</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1330</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" s="0"/>
@@ -14042,7 +14002,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -14071,31 +14031,31 @@
         <v>689</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>1333</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>1334</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>1335</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>1337</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>1338</v>
       </c>
     </row>
   </sheetData>
@@ -14128,10 +14088,10 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="B1" s="5" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1339</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1340</v>
       </c>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
@@ -14144,13 +14104,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>1341</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1341</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1342</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
@@ -14160,7 +14120,7 @@
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="W2" s="5" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14189,7 +14149,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0"/>
@@ -14203,7 +14163,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0"/>
@@ -14217,7 +14177,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
@@ -14231,7 +14191,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
@@ -14240,18 +14200,18 @@
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="J8" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>1348</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
@@ -14260,21 +14220,21 @@
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="J9" s="5" t="s">
+        <v>1350</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>1351</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>1352</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>1353</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>1354</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1355</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
@@ -14282,18 +14242,18 @@
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="J10" s="5" t="s">
+        <v>1355</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>1356</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>1357</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>1358</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -14302,18 +14262,18 @@
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="J11" s="5" t="s">
+        <v>1359</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>1360</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>1361</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>1362</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
@@ -14322,21 +14282,21 @@
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="J12" s="5" t="s">
+        <v>1363</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>1364</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>1365</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>1366</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>1367</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>1368</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
@@ -14344,21 +14304,21 @@
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="J13" s="5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>1369</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>1370</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>1371</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>1372</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>1373</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
@@ -14367,10 +14327,10 @@
       <c r="G14" s="0"/>
       <c r="J14" s="0"/>
       <c r="L14" s="5" t="s">
+        <v>1373</v>
+      </c>
+      <c r="M14" s="5" t="s">
         <v>1374</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14387,7 +14347,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -14396,13 +14356,13 @@
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="J16" s="5" t="s">
+        <v>1376</v>
+      </c>
+      <c r="L16" s="5" t="s">
         <v>1377</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>1378</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>1379</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14414,18 +14374,18 @@
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="J17" s="5" t="s">
+        <v>1379</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>1380</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>1381</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>1382</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -14434,15 +14394,15 @@
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="J18" s="5" t="s">
+        <v>1383</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>1384</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>1385</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
@@ -14451,7 +14411,7 @@
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
       <c r="J19" s="5" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="L19" s="0"/>
     </row>
@@ -14467,7 +14427,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -14489,7 +14449,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -14501,10 +14461,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>1390</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>1391</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
@@ -14512,7 +14472,7 @@
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
       <c r="L24" s="5" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14524,15 +14484,15 @@
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
       <c r="L25" s="5" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>1394</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>1395</v>
       </c>
       <c r="C26" s="0"/>
       <c r="D26" s="0"/>
@@ -14540,7 +14500,7 @@
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
       <c r="L26" s="5" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14552,12 +14512,12 @@
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="L27" s="5" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
@@ -14566,7 +14526,7 @@
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
       <c r="L28" s="5" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14588,7 +14548,7 @@
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
       <c r="L30" s="5" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14600,7 +14560,7 @@
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="L31" s="5" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14612,7 +14572,7 @@
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
       <c r="L32" s="5" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14624,7 +14584,7 @@
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="L33" s="5" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14636,38 +14596,38 @@
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>
       <c r="L34" s="5" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>1343</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>1345</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>1344</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>1405</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="L35" s="5" t="s">
         <v>1406</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>1407</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L36" s="5" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
   </sheetData>
@@ -14702,15 +14662,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1410</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1411</v>
       </c>
     </row>
   </sheetData>
@@ -14745,10 +14705,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1412</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1413</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14756,7 +14716,7 @@
         <v>613</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>609</v>
@@ -14764,10 +14724,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>1415</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1416</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>196</v>
@@ -14775,10 +14735,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>1417</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1418</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>196</v>
@@ -14786,18 +14746,18 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>1419</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1420</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>1421</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1422</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14805,7 +14765,7 @@
         <v>776</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14813,7 +14773,7 @@
         <v>806</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14821,7 +14781,7 @@
         <v>964</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14829,7 +14789,7 @@
         <v>1025</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14837,7 +14797,7 @@
         <v>1046</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14845,7 +14805,7 @@
         <v>1098</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14853,23 +14813,23 @@
         <v>1118</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>1430</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>1431</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>1432</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>1433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added carangan character pages and corrected spelling mistakes in the main description page
</commit_message>
<xml_diff>
--- a/input/characters.xlsx
+++ b/input/characters.xlsx
@@ -3865,7 +3865,7 @@
     <t xml:space="preserve">Mustikawati:x</t>
   </si>
   <si>
-    <t xml:space="preserve">Missing pages!</t>
+    <t xml:space="preserve">592-594</t>
   </si>
   <si>
     <t xml:space="preserve">242-245 (Vol. IX)</t>
@@ -4794,7 +4794,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4911,10 +4911,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4999,44 +4995,44 @@
   <dimension ref="A1:AC148"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T139" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
+      <selection pane="bottomRight" activeCell="T141" activeCellId="0" sqref="T141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.1683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.4438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.3724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="51.0816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="41.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="42.4438775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="44.9234693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="82.9387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="134.454081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="53.5663265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="41.7959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="33.3724489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="46.0051020408163"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="35.530612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="51.0816326530612"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="79.0510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="20.734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="28.5102040816327"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="38.5561224489796"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="62.8520408163265"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="54.2142857142857"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="77.969387755102"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="74.1938775510204"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="70.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.9234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.9081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="51.9438775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="41.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="43.0918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="45.5714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="84.3418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="136.719387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="54.4285714285714"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="42.4438775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="33.9081632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="46.7602040816327"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="51.9438775510204"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="80.3469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="29.0510204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="39.2040816326531"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="63.9336734693878"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="55.0765306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="79.265306122449"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="75.4897959183674"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="71.8163265306122"/>
     <col collapsed="false" hidden="false" max="1023" min="30" style="1" width="5.83163265306122"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="3" width="5.83163265306122"/>
   </cols>
@@ -12879,7 +12875,7 @@
       <c r="P141" s="0"/>
       <c r="Q141" s="5"/>
       <c r="S141" s="0"/>
-      <c r="T141" s="29" t="s">
+      <c r="T141" s="2" t="s">
         <v>1199</v>
       </c>
       <c r="U141" s="2" t="n">
@@ -12971,7 +12967,7 @@
       <c r="F143" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="G143" s="30" t="s">
+      <c r="G143" s="29" t="s">
         <v>1216</v>
       </c>
       <c r="H143" s="1" t="s">
@@ -13014,7 +13010,7 @@
       <c r="F144" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="G144" s="30" t="s">
+      <c r="G144" s="29" t="s">
         <v>1220</v>
       </c>
       <c r="H144" s="1" t="s">
@@ -13253,7 +13249,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13335,12 +13331,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="45.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="43.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="103.887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="61.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="103.887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="46.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="44.6020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="105.617346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="62.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="105.617346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13916,7 +13912,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="42.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="43.0918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14078,7 +14074,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="66.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="67.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14650,7 +14646,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="15.1173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14693,7 +14689,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="15.3367346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14852,7 +14848,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.3571428571429"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14878,7 +14874,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.3571428571429"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14904,7 +14900,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="22.3571428571429"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>